<commit_message>
commit and push premier changes
</commit_message>
<xml_diff>
--- a/src/main/resources/testdesign/testcontroller/master.xlsx
+++ b/src/main/resources/testdesign/testcontroller/master.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4F30ED4D-2080-4198-AE1C-FBE57AB9BE8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{269DD782-E083-495D-ACF2-79195DE91070}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="App_Info" sheetId="1" r:id="rId1"/>
@@ -1453,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC91813-AD9F-4B65-8DAD-DE1B79C09543}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B76D93-F2C0-4CD2-AA8C-AD315425546C}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
commit and Push changes
</commit_message>
<xml_diff>
--- a/src/main/resources/testdesign/testcontroller/master.xlsx
+++ b/src/main/resources/testdesign/testcontroller/master.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiservcorp-my.sharepoint.com/personal/moksha_mukh_fiserv_com/Documents/Desktop/Republic UAT/TestAutomation/git/workspace/Test_Automation/src/main/resources/testdesign/testcontroller/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FARK7SF\Desktop\Republic UAT\Git\workspace\Test_Automation\src\main\resources\testdesign\testcontroller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{4F30ED4D-2080-4198-AE1C-FBE57AB9BE8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7854ED11-C6A0-40E7-A04B-873F85C2D56A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299391E0-8BE4-4C8C-BE58-65CA9E77E00F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="170">
   <si>
     <t>Application_Name</t>
   </si>
@@ -1862,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B76D93-F2C0-4CD2-AA8C-AD315425546C}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,7 +2159,7 @@
         <v>118</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -2307,7 +2307,9 @@
       <c r="A19" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="B19" s="15"/>
+      <c r="B19" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -2323,7 +2325,9 @@
       <c r="A20" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -2339,7 +2343,9 @@
       <c r="A21" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -2355,7 +2361,9 @@
       <c r="A22" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B22" s="15"/>
+      <c r="B22" s="15" t="s">
+        <v>5</v>
+      </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>

</xml_diff>

<commit_message>
My changes on CC
</commit_message>
<xml_diff>
--- a/src/main/resources/testdesign/testcontroller/master.xlsx
+++ b/src/main/resources/testdesign/testcontroller/master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FARK7SF\Desktop\Republic UAT\Git\workspace\Test_Automation\src\main\resources\testdesign\testcontroller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New_FrameWork\Git\Workspace\Test_Automation\src\main\resources\testdesign\testcontroller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299391E0-8BE4-4C8C-BE58-65CA9E77E00F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20305BAC-C33D-4B9D-8EFA-6CA0D414AE78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="App_Info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -29,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="231">
   <si>
     <t>Application_Name</t>
   </si>
@@ -558,11 +557,205 @@
   <si>
     <t>Premier_TC020</t>
   </si>
+  <si>
+    <t>sthangapalam</t>
+  </si>
+  <si>
+    <t>'2021/11/30 19:14:11</t>
+  </si>
+  <si>
+    <t>'2021/11/30 19:16:35</t>
+  </si>
+  <si>
+    <t>'2021/11/30 19:49:25</t>
+  </si>
+  <si>
+    <t>'2021/11/30 20:08:23</t>
+  </si>
+  <si>
+    <t>'2021/12/01 13:56:45</t>
+  </si>
+  <si>
+    <t>'2021/12/01 14:18:20</t>
+  </si>
+  <si>
+    <t>EPP_TC001_01</t>
+  </si>
+  <si>
+    <t>EPP_TC012_01</t>
+  </si>
+  <si>
+    <t>'2021/12/01 14:48:20</t>
+  </si>
+  <si>
+    <t>'2021/12/01 15:09:52</t>
+  </si>
+  <si>
+    <t>'2021/12/01 15:26:03</t>
+  </si>
+  <si>
+    <t>'2021/12/03 11:17:58</t>
+  </si>
+  <si>
+    <t>'2021/12/03 11:20:10</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC012</t>
+  </si>
+  <si>
+    <t>Create a batch template and search it
+(flexbile to add 1 to any number of payees)</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC013</t>
+  </si>
+  <si>
+    <t>Edit a batch template and Seach it
+if Existing template , do a edit
+else create new template and do edit</t>
+  </si>
+  <si>
+    <t>'2021/12/16 12:04:44</t>
+  </si>
+  <si>
+    <t>'2021/12/16 12:13:43</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC014</t>
+  </si>
+  <si>
+    <t>Initiate Ach Payment using batch template- Approval
+if Existing template , do a payment activity
+elseCreate batch template, use that template and do payments</t>
+  </si>
+  <si>
+    <t>'2021/12/21 00:13:42</t>
+  </si>
+  <si>
+    <t>'2021/12/21 00:25:44</t>
+  </si>
+  <si>
+    <t>Initiate Ach Payment using batch template- Reject
+if Existing template , do a payment activity
+elseCreate batch template, use that template and do payments</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC015</t>
+  </si>
+  <si>
+    <t>'2021/12/21 01:14:00</t>
+  </si>
+  <si>
+    <t>'2021/12/21 01:21:13</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC016</t>
+  </si>
+  <si>
+    <t>Initiate Ach Payment using batch template- Cancel
+if Existing template , do a payment activity
+elseCreate batch template, use that template and do payments</t>
+  </si>
+  <si>
+    <t>'2021/12/21 15:31:44</t>
+  </si>
+  <si>
+    <t>'2021/12/21 15:38:37</t>
+  </si>
+  <si>
+    <t>'2021/12/21 16:17:50</t>
+  </si>
+  <si>
+    <t>'2021/12/21 16:29:20</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC020</t>
+  </si>
+  <si>
+    <t>Create a confidential batch template and search it
+(flexbile to add 1 to any number of payees)</t>
+  </si>
+  <si>
+    <t>'2021/12/21 18:51:15</t>
+  </si>
+  <si>
+    <t>'2021/12/21 19:05:08</t>
+  </si>
+  <si>
+    <t>'2021/12/22 16:56:10</t>
+  </si>
+  <si>
+    <t>'2021/12/22 17:15:05</t>
+  </si>
+  <si>
+    <t>'2021/12/23 16:53:46</t>
+  </si>
+  <si>
+    <t>'2021/12/23 16:56:12</t>
+  </si>
+  <si>
+    <t>'2021/12/23 19:31:45</t>
+  </si>
+  <si>
+    <t>'2021/12/23 19:39:36</t>
+  </si>
+  <si>
+    <t>'2021/12/23 21:35:20</t>
+  </si>
+  <si>
+    <t>'2021/12/23 21:42:51</t>
+  </si>
+  <si>
+    <t>'2021/12/23 21:48:42</t>
+  </si>
+  <si>
+    <t>'2021/12/23 21:58:14</t>
+  </si>
+  <si>
+    <t>'2021/12/24 12:27:18</t>
+  </si>
+  <si>
+    <t>'2021/12/24 12:39:16</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC017</t>
+  </si>
+  <si>
+    <t>Initiate Ach Payment using free form- Approval</t>
+  </si>
+  <si>
+    <t>'2022/01/03 12:58:15</t>
+  </si>
+  <si>
+    <t>'2022/01/03 13:01:06</t>
+  </si>
+  <si>
+    <t>'2022/01/03 17:22:57</t>
+  </si>
+  <si>
+    <t>'2022/01/03 17:29:38</t>
+  </si>
+  <si>
+    <t>'2022/01/03 17:42:48</t>
+  </si>
+  <si>
+    <t>'2022/01/03 17:48:05</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>'2022/01/04 16:47:04</t>
+  </si>
+  <si>
+    <t>'2022/01/04 17:00:57</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1083,15 +1276,15 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="49.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1138,7 +1331,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1152,7 +1345,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
@@ -1174,23 +1367,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5698D2-2A68-44BF-B3E0-84682E6FAE93}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="79" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="63.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="63.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1236,7 +1429,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1265,7 +1458,7 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -1380,6 +1573,18 @@
       <c r="F7" t="s">
         <v>38</v>
       </c>
+      <c r="H7" t="s">
+        <v>170</v>
+      </c>
+      <c r="I7" t="s">
+        <v>210</v>
+      </c>
+      <c r="J7" t="s">
+        <v>211</v>
+      </c>
+      <c r="K7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1397,6 +1602,18 @@
       <c r="F8" t="s">
         <v>40</v>
       </c>
+      <c r="H8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J8" t="s">
+        <v>215</v>
+      </c>
+      <c r="K8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1414,6 +1631,18 @@
       <c r="F9" t="s">
         <v>42</v>
       </c>
+      <c r="H9" t="s">
+        <v>170</v>
+      </c>
+      <c r="I9" t="s">
+        <v>214</v>
+      </c>
+      <c r="J9" t="s">
+        <v>216</v>
+      </c>
+      <c r="K9" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1431,6 +1660,18 @@
       <c r="F10" t="s">
         <v>44</v>
       </c>
+      <c r="H10" t="s">
+        <v>170</v>
+      </c>
+      <c r="I10" t="s">
+        <v>208</v>
+      </c>
+      <c r="J10" t="s">
+        <v>209</v>
+      </c>
+      <c r="K10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1448,6 +1689,18 @@
       <c r="F11" t="s">
         <v>47</v>
       </c>
+      <c r="H11" t="s">
+        <v>170</v>
+      </c>
+      <c r="I11" t="s">
+        <v>212</v>
+      </c>
+      <c r="J11" t="s">
+        <v>213</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1465,6 +1718,18 @@
       <c r="F12" t="s">
         <v>49</v>
       </c>
+      <c r="H12" t="s">
+        <v>170</v>
+      </c>
+      <c r="I12" t="s">
+        <v>214</v>
+      </c>
+      <c r="J12" t="s">
+        <v>217</v>
+      </c>
+      <c r="K12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1482,6 +1747,18 @@
       <c r="F13" s="9" t="s">
         <v>61</v>
       </c>
+      <c r="H13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" t="s">
+        <v>218</v>
+      </c>
+      <c r="J13" t="s">
+        <v>219</v>
+      </c>
+      <c r="K13" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1499,6 +1776,18 @@
       <c r="F14" s="9" t="s">
         <v>52</v>
       </c>
+      <c r="H14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I14" t="s">
+        <v>222</v>
+      </c>
+      <c r="J14" t="s">
+        <v>223</v>
+      </c>
+      <c r="K14" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1516,6 +1805,18 @@
       <c r="F15" s="9" t="s">
         <v>63</v>
       </c>
+      <c r="H15" t="s">
+        <v>170</v>
+      </c>
+      <c r="I15" t="s">
+        <v>224</v>
+      </c>
+      <c r="J15" t="s">
+        <v>225</v>
+      </c>
+      <c r="K15" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1533,8 +1834,20 @@
       <c r="F16" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>170</v>
+      </c>
+      <c r="I16" t="s">
+        <v>226</v>
+      </c>
+      <c r="J16" t="s">
+        <v>227</v>
+      </c>
+      <c r="K16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -1549,6 +1862,209 @@
       </c>
       <c r="F17" s="9" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H18" t="s">
+        <v>170</v>
+      </c>
+      <c r="I18" t="s">
+        <v>202</v>
+      </c>
+      <c r="J18" t="s">
+        <v>203</v>
+      </c>
+      <c r="K18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="H19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" t="s">
+        <v>188</v>
+      </c>
+      <c r="J19" t="s">
+        <v>189</v>
+      </c>
+      <c r="K19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J20" t="s">
+        <v>193</v>
+      </c>
+      <c r="K20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="H21" t="s">
+        <v>170</v>
+      </c>
+      <c r="I21" t="s">
+        <v>196</v>
+      </c>
+      <c r="J21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>198</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="H22" t="s">
+        <v>170</v>
+      </c>
+      <c r="I22" t="s">
+        <v>200</v>
+      </c>
+      <c r="J22" t="s">
+        <v>201</v>
+      </c>
+      <c r="K22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="H23" t="s">
+        <v>170</v>
+      </c>
+      <c r="I23" t="s">
+        <v>229</v>
+      </c>
+      <c r="J23" t="s">
+        <v>230</v>
+      </c>
+      <c r="K23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="H24" t="s">
+        <v>170</v>
+      </c>
+      <c r="I24" t="s">
+        <v>206</v>
+      </c>
+      <c r="J24" t="s">
+        <v>207</v>
+      </c>
+      <c r="K24" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1559,22 +2075,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC91813-AD9F-4B65-8DAD-DE1B79C09543}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="43.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="11" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="104.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1617,7 +2134,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1771,7 +2288,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -1781,6 +2298,18 @@
       </c>
       <c r="F13" t="s">
         <v>135</v>
+      </c>
+      <c r="H13" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J13" t="s">
+        <v>176</v>
+      </c>
+      <c r="K13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1824,8 +2353,20 @@
       <c r="F16" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>170</v>
+      </c>
+      <c r="I16" t="s">
+        <v>173</v>
+      </c>
+      <c r="J16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>142</v>
       </c>
@@ -1839,18 +2380,70 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>144</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
         <v>145</v>
       </c>
       <c r="F18" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" t="s">
+        <v>179</v>
+      </c>
+      <c r="J19" t="s">
+        <v>180</v>
+      </c>
+      <c r="K19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" t="s">
+        <v>170</v>
+      </c>
+      <c r="I20" t="s">
+        <v>179</v>
+      </c>
+      <c r="J20" t="s">
+        <v>181</v>
+      </c>
+      <c r="K20" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1862,22 +2455,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B76D93-F2C0-4CD2-AA8C-AD315425546C}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="73.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="73.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2263,7 +2856,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
     </row>
-    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>127</v>
       </c>
@@ -2283,7 +2876,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>129</v>
       </c>
@@ -2303,12 +2896,12 @@
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>166</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -2317,11 +2910,20 @@
         <v>162</v>
       </c>
       <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" t="s">
+        <v>182</v>
+      </c>
+      <c r="J19" t="s">
+        <v>183</v>
+      </c>
+      <c r="K19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>167</v>
       </c>
@@ -2339,7 +2941,7 @@
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>168</v>
       </c>
@@ -2357,12 +2959,12 @@
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
     </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>169</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -2371,9 +2973,18 @@
         <v>165</v>
       </c>
       <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
+      <c r="H22" t="s">
+        <v>170</v>
+      </c>
+      <c r="I22" t="s">
+        <v>171</v>
+      </c>
+      <c r="J22" t="s">
+        <v>172</v>
+      </c>
+      <c r="K22" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Master Sheet updated 1/19
</commit_message>
<xml_diff>
--- a/src/main/resources/testdesign/testcontroller/master.xlsx
+++ b/src/main/resources/testdesign/testcontroller/master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New_FrameWork\Git\Workspace\Test_Automation\src\main\resources\testdesign\testcontroller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiservcorp-my.sharepoint.com/personal/moksha_mukh_fiserv_com/Documents/Desktop/Republic UAT/TestAutomation/git/workspace/Test_Automation/src/main/resources/testdesign/testcontroller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414AA4E1-2F53-4458-9B23-2B82D433B8FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{DAF2207D-6EEF-4B6A-A45F-E4DA9721D19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D6BFA59-14EE-48C2-8F31-DDFD2672A36B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Premier" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Premier!$A$1:$L$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Premier!$A$1:$L$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,6 +32,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="527">
   <si>
     <t>Application_Name</t>
   </si>
@@ -302,15 +303,6 @@
     <t>TC010</t>
   </si>
   <si>
-    <t>'2021/11/17 22:19:06</t>
-  </si>
-  <si>
-    <t>'2021/11/17 22:21:20</t>
-  </si>
-  <si>
-    <t>'2021/11/17 22:21:58</t>
-  </si>
-  <si>
     <t>'2021/11/18 13:34:38</t>
   </si>
   <si>
@@ -821,48 +813,6 @@
     <t>TC075</t>
   </si>
   <si>
-    <t>Premier_TC076</t>
-  </si>
-  <si>
-    <t>TC076</t>
-  </si>
-  <si>
-    <t>Premier_TC077</t>
-  </si>
-  <si>
-    <t>TC077</t>
-  </si>
-  <si>
-    <t>Premier_TC078</t>
-  </si>
-  <si>
-    <t>TC078</t>
-  </si>
-  <si>
-    <t>Premier_TC079</t>
-  </si>
-  <si>
-    <t>TC079</t>
-  </si>
-  <si>
-    <t>Premier_TC080</t>
-  </si>
-  <si>
-    <t>TC080</t>
-  </si>
-  <si>
-    <t>Premier_TC081</t>
-  </si>
-  <si>
-    <t>TC081</t>
-  </si>
-  <si>
-    <t>Premier_TC082</t>
-  </si>
-  <si>
-    <t>TC082</t>
-  </si>
-  <si>
     <t>'2021/12/22 11:01:11</t>
   </si>
   <si>
@@ -956,9 +906,6 @@
     <t>Create a Demand deposit Account for individual customers(Search Customer)</t>
   </si>
   <si>
-    <t xml:space="preserve">Update  Saving account </t>
-  </si>
-  <si>
     <t>Create a Certificate  Account for individual customers</t>
   </si>
   <si>
@@ -968,9 +915,6 @@
     <t>Create a Certificate  Account for individual customers(Search Customer)</t>
   </si>
   <si>
-    <t>Update  Certificate  account</t>
-  </si>
-  <si>
     <t>Create a Loan Account for individual customers</t>
   </si>
   <si>
@@ -1049,15 +993,6 @@
     <t>DD-DD account maintenance update overdrafts</t>
   </si>
   <si>
-    <t>DD-DD account maintenance add new relationship</t>
-  </si>
-  <si>
-    <t>DD-DD account maintenance update relationship</t>
-  </si>
-  <si>
-    <t>DD-DD account maintenance remove relationship</t>
-  </si>
-  <si>
     <t>DD-DD account maintenance update status</t>
   </si>
   <si>
@@ -1067,18 +1002,9 @@
     <t>DD-DD account maintenance update codes -statement notifications</t>
   </si>
   <si>
-    <t>Savings-Savings account maintenance update Tickler</t>
-  </si>
-  <si>
     <t>Savings-Savings account maintenance update hold</t>
   </si>
   <si>
-    <t>Savings-Savings account maintenance Savings add new relationship</t>
-  </si>
-  <si>
-    <t>Savings-Savings account maintenance update relationship</t>
-  </si>
-  <si>
     <t>Savings-Savings account maintenance remove relationship</t>
   </si>
   <si>
@@ -1091,24 +1017,12 @@
     <t>Savings-Savings account maintenance update codes statement notification</t>
   </si>
   <si>
-    <t>Certificates-Certificates account maintenance update Tickler</t>
-  </si>
-  <si>
     <t>Certificates-Certificates account maintenance update hold</t>
   </si>
   <si>
-    <t>Certificates-Certificates account maintenance Certificates add new relationship</t>
-  </si>
-  <si>
     <t>Certificates-Certificates account maintenance update status</t>
   </si>
   <si>
-    <t>Certificates-Certificates account maintenance update relationship</t>
-  </si>
-  <si>
-    <t>Certificates-Certificates account maintenance remove relationship</t>
-  </si>
-  <si>
     <t xml:space="preserve">Certificates-Certificates account maintenance update codes - statement notiifcation </t>
   </si>
   <si>
@@ -1130,55 +1044,22 @@
     <t>'2021/12/22 23:08:23</t>
   </si>
   <si>
-    <t>'2021/12/22 23:55:54</t>
-  </si>
-  <si>
-    <t>'2021/12/23 00:16:25</t>
-  </si>
-  <si>
     <t>'2021/12/23 00:20:26</t>
   </si>
   <si>
-    <t>'2021/12/23 00:23:18</t>
-  </si>
-  <si>
-    <t>'2021/12/23 00:26:04</t>
-  </si>
-  <si>
-    <t>'2021/12/23 00:29:23</t>
-  </si>
-  <si>
     <t>'2021/12/23 00:33:31</t>
   </si>
   <si>
-    <t>'2021/12/23 00:36:16</t>
-  </si>
-  <si>
-    <t>'2021/12/23 00:39:29</t>
-  </si>
-  <si>
-    <t>'2021/12/23 00:43:04</t>
-  </si>
-  <si>
     <t>'2021/12/23 21:57:38</t>
   </si>
   <si>
     <t>'2021/12/23 21:59:24</t>
   </si>
   <si>
-    <t>'2021/12/23 22:05:53</t>
-  </si>
-  <si>
     <t>'2021/12/23 22:09:54</t>
   </si>
   <si>
     <t>'2021/12/24 13:16:20</t>
-  </si>
-  <si>
-    <t>'2021/12/24 13:21:22</t>
-  </si>
-  <si>
-    <t>'2021/12/24 13:26:25</t>
   </si>
   <si>
     <t>'2021/12/24 13:31:48</t>
@@ -1455,6 +1336,138 @@
     <t>'2021/12/21 19:05:08</t>
   </si>
   <si>
+    <t>ExecutionStatus_5</t>
+  </si>
+  <si>
+    <t>ExecutionStatus_6</t>
+  </si>
+  <si>
+    <t>ExecutionStatus_7</t>
+  </si>
+  <si>
+    <t>ExecutionStatus_8</t>
+  </si>
+  <si>
+    <t>ExecutionStatus_9</t>
+  </si>
+  <si>
+    <t>ExecutionStatus_10</t>
+  </si>
+  <si>
+    <t>'2022/01/06 16:40:34</t>
+  </si>
+  <si>
+    <t>'2022/01/06 16:54:54</t>
+  </si>
+  <si>
+    <t>'2022/01/06 20:33:14</t>
+  </si>
+  <si>
+    <t>'2022/01/06 20:36:38</t>
+  </si>
+  <si>
+    <t>'2022/01/04 22:54:31</t>
+  </si>
+  <si>
+    <t>'2022/01/05 00:52:18</t>
+  </si>
+  <si>
+    <t>'2022/01/05 01:40:51</t>
+  </si>
+  <si>
+    <t>'2022/01/05 01:59:16</t>
+  </si>
+  <si>
+    <t>'2022/01/05 02:44:34</t>
+  </si>
+  <si>
+    <t>'2022/01/05 03:36:14</t>
+  </si>
+  <si>
+    <t>'2022/01/05 03:54:39</t>
+  </si>
+  <si>
+    <t>'2022/01/05 04:50:43</t>
+  </si>
+  <si>
+    <t>'2022/01/05 19:28:39</t>
+  </si>
+  <si>
+    <t>'2022/01/05 19:32:47</t>
+  </si>
+  <si>
+    <t>'2022/01/06 15:59:57</t>
+  </si>
+  <si>
+    <t>'2022/01/06 16:13:01</t>
+  </si>
+  <si>
+    <t>'2022/01/06 19:05:13</t>
+  </si>
+  <si>
+    <t>'2022/01/06 19:08:43</t>
+  </si>
+  <si>
+    <t>DD-DD account maintenance Stop Payments</t>
+  </si>
+  <si>
+    <t>DD-DD account maintenance add new/update relationship</t>
+  </si>
+  <si>
+    <t>'2022/01/10 22:35:22</t>
+  </si>
+  <si>
+    <t>'2022/01/10 22:37:25</t>
+  </si>
+  <si>
+    <t>'2022/01/10 22:39:32</t>
+  </si>
+  <si>
+    <t>'2022/01/10 23:17:04</t>
+  </si>
+  <si>
+    <t>'2022/01/10 23:18:51</t>
+  </si>
+  <si>
+    <t>'2022/01/11 14:28:36</t>
+  </si>
+  <si>
+    <t>'2022/01/11 14:30:27</t>
+  </si>
+  <si>
+    <t>'2022/01/12 13:36:57</t>
+  </si>
+  <si>
+    <t>'2022/01/12 13:40:03</t>
+  </si>
+  <si>
+    <t>Savings-Savings account maintenance Stop Payments</t>
+  </si>
+  <si>
+    <t>Update  Saving account with warnings</t>
+  </si>
+  <si>
+    <t>Update  Certificate  account with warnings</t>
+  </si>
+  <si>
+    <t>'2022/01/12 19:45:22</t>
+  </si>
+  <si>
+    <t>'2022/01/12 19:47:53</t>
+  </si>
+  <si>
+    <t>'2022/01/12 19:49:00</t>
+  </si>
+  <si>
+    <t>'2021/11/17 22:19:06</t>
+  </si>
+  <si>
+    <t>'2021/11/17 22:21:20</t>
+  </si>
+  <si>
+    <t>'2021/11/17 22:21:58</t>
+  </si>
+  <si>
     <t>CC_CORP_TC018</t>
   </si>
   <si>
@@ -1535,9 +1548,6 @@
     <t>'2022/01/07 13:58:23</t>
   </si>
   <si>
-    <t>https://portal.cert.fec-frms.fiservapps.com/portal/login?c=D010019</t>
-  </si>
-  <si>
     <t>CC_CORP_TC025</t>
   </si>
   <si>
@@ -1562,6 +1572,69 @@
   </si>
   <si>
     <t>'2022/01/12 14:46:06</t>
+  </si>
+  <si>
+    <t>'2022/01/12 22:12:40</t>
+  </si>
+  <si>
+    <t>'2022/01/12 22:15:02</t>
+  </si>
+  <si>
+    <t>https://portal.cert.fec-frms.fiservapps.com/portal/login?c=D010019</t>
+  </si>
+  <si>
+    <t>'2022/01/13 19:43:01</t>
+  </si>
+  <si>
+    <t>'2022/01/13 19:53:41</t>
+  </si>
+  <si>
+    <t>'2022/01/13 22:01:14</t>
+  </si>
+  <si>
+    <t>'2022/01/13 22:05:29</t>
+  </si>
+  <si>
+    <t>'2022/01/14 08:38:46</t>
+  </si>
+  <si>
+    <t>'2022/01/14 08:41:38</t>
+  </si>
+  <si>
+    <t>'2022/01/14 09:43:22</t>
+  </si>
+  <si>
+    <t>'2022/01/14 09:55:02</t>
+  </si>
+  <si>
+    <t>'2022/01/14 10:23:21</t>
+  </si>
+  <si>
+    <t>'2022/01/14 10:33:54</t>
+  </si>
+  <si>
+    <t>'2022/01/14 15:37:39</t>
+  </si>
+  <si>
+    <t>'2022/01/14 15:43:25</t>
+  </si>
+  <si>
+    <t>'2022/01/14 15:45:25</t>
+  </si>
+  <si>
+    <t>'2022/01/14 15:57:59</t>
+  </si>
+  <si>
+    <t>'2022/01/14 16:44:49</t>
+  </si>
+  <si>
+    <t>'2022/01/14 17:03:27</t>
+  </si>
+  <si>
+    <t>'2022/01/14 17:09:28</t>
+  </si>
+  <si>
+    <t>'2022/01/14 17:23:23</t>
   </si>
   <si>
     <t>CC_CORP_TC027</t>
@@ -1618,7 +1691,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1628,6 +1701,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1814,16 +1893,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2108,7 +2185,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,13 +2215,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>492</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2163,7 +2240,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -2183,18 +2260,17 @@
         <v>67</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{4D28C060-3FC7-4384-B377-95BDC209822A}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{E2A5E61D-28EC-4233-AFA8-278DC779E7DC}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{2A8B23C1-C7BA-47E8-B0D7-206F6F1578A8}"/>
-    <hyperlink ref="E2" r:id="rId4" tooltip="https://portal.cert.fec-frms.fiservapps.com/portal/login?c=d010019" xr:uid="{C2F5B005-8811-4AAA-9A78-6DA23B925BF2}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{795D2318-ED88-4911-BD2D-6C2865044338}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{2A8B23C1-C7BA-47E8-B0D7-206F6F1578A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2202,14 +2278,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5698D2-2A68-44BF-B3E0-84682E6FAE93}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:K16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="79" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="63.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -2277,10 +2353,10 @@
         <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K2" t="s">
         <v>70</v>
@@ -2306,10 +2382,10 @@
         <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K3" t="s">
         <v>70</v>
@@ -2335,10 +2411,10 @@
         <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>87</v>
+        <v>469</v>
       </c>
       <c r="J4" t="s">
-        <v>88</v>
+        <v>470</v>
       </c>
       <c r="K4" t="s">
         <v>70</v>
@@ -2364,10 +2440,10 @@
         <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>87</v>
+        <v>469</v>
       </c>
       <c r="J5" t="s">
-        <v>89</v>
+        <v>471</v>
       </c>
       <c r="K5" t="s">
         <v>70</v>
@@ -2407,13 +2483,13 @@
         <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I7" t="s">
-        <v>422</v>
+        <v>382</v>
       </c>
       <c r="J7" t="s">
-        <v>423</v>
+        <v>383</v>
       </c>
       <c r="K7" t="s">
         <v>70</v>
@@ -2436,13 +2512,13 @@
         <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I8" t="s">
-        <v>424</v>
+        <v>384</v>
       </c>
       <c r="J8" t="s">
-        <v>425</v>
+        <v>385</v>
       </c>
       <c r="K8" t="s">
         <v>70</v>
@@ -2465,13 +2541,13 @@
         <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I9" t="s">
-        <v>424</v>
+        <v>384</v>
       </c>
       <c r="J9" t="s">
-        <v>426</v>
+        <v>386</v>
       </c>
       <c r="K9" t="s">
         <v>70</v>
@@ -2494,13 +2570,13 @@
         <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I10" t="s">
-        <v>427</v>
+        <v>387</v>
       </c>
       <c r="J10" t="s">
-        <v>428</v>
+        <v>388</v>
       </c>
       <c r="K10" t="s">
         <v>70</v>
@@ -2523,13 +2599,13 @@
         <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I11" t="s">
-        <v>429</v>
+        <v>389</v>
       </c>
       <c r="J11" t="s">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="K11" t="s">
         <v>70</v>
@@ -2552,13 +2628,13 @@
         <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I12" t="s">
-        <v>424</v>
+        <v>384</v>
       </c>
       <c r="J12" t="s">
-        <v>431</v>
+        <v>391</v>
       </c>
       <c r="K12" t="s">
         <v>70</v>
@@ -2581,13 +2657,13 @@
         <v>60</v>
       </c>
       <c r="H13" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I13" t="s">
-        <v>432</v>
+        <v>392</v>
       </c>
       <c r="J13" t="s">
-        <v>433</v>
+        <v>393</v>
       </c>
       <c r="K13" t="s">
         <v>70</v>
@@ -2610,13 +2686,13 @@
         <v>52</v>
       </c>
       <c r="H14" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I14" t="s">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="J14" t="s">
-        <v>435</v>
+        <v>395</v>
       </c>
       <c r="K14" t="s">
         <v>70</v>
@@ -2639,13 +2715,13 @@
         <v>62</v>
       </c>
       <c r="H15" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I15" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="J15" t="s">
-        <v>437</v>
+        <v>397</v>
       </c>
       <c r="K15" t="s">
         <v>70</v>
@@ -2668,16 +2744,16 @@
         <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I16" t="s">
-        <v>438</v>
+        <v>398</v>
       </c>
       <c r="J16" t="s">
-        <v>439</v>
+        <v>399</v>
       </c>
       <c r="K16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2699,7 +2775,7 @@
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>440</v>
+        <v>400</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -2708,19 +2784,19 @@
         <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>440</v>
+        <v>400</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>441</v>
+        <v>401</v>
       </c>
       <c r="H18" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I18" t="s">
-        <v>442</v>
+        <v>402</v>
       </c>
       <c r="J18" t="s">
-        <v>443</v>
+        <v>403</v>
       </c>
       <c r="K18" t="s">
         <v>70</v>
@@ -2728,7 +2804,7 @@
     </row>
     <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -2737,19 +2813,19 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>445</v>
+        <v>405</v>
       </c>
       <c r="H19" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I19" t="s">
-        <v>446</v>
+        <v>406</v>
       </c>
       <c r="J19" t="s">
-        <v>447</v>
+        <v>407</v>
       </c>
       <c r="K19" t="s">
         <v>70</v>
@@ -2757,7 +2833,7 @@
     </row>
     <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -2766,19 +2842,19 @@
         <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>448</v>
+        <v>408</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
       <c r="H20" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I20" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
       <c r="J20" t="s">
-        <v>451</v>
+        <v>411</v>
       </c>
       <c r="K20" t="s">
         <v>70</v>
@@ -2786,7 +2862,7 @@
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -2795,19 +2871,19 @@
         <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>452</v>
+        <v>412</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="H21" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I21" t="s">
-        <v>454</v>
+        <v>414</v>
       </c>
       <c r="J21" t="s">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="K21" t="s">
         <v>70</v>
@@ -2815,7 +2891,7 @@
     </row>
     <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -2824,19 +2900,19 @@
         <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>456</v>
+        <v>416</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="H22" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I22" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="J22" t="s">
-        <v>459</v>
+        <v>419</v>
       </c>
       <c r="K22" t="s">
         <v>70</v>
@@ -2844,7 +2920,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -2853,19 +2929,19 @@
         <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>460</v>
+        <v>420</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>461</v>
+        <v>421</v>
       </c>
       <c r="H23" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I23" t="s">
-        <v>462</v>
+        <v>422</v>
       </c>
       <c r="J23" t="s">
-        <v>463</v>
+        <v>423</v>
       </c>
       <c r="K23" t="s">
         <v>70</v>
@@ -2873,7 +2949,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -2882,19 +2958,19 @@
         <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="H24" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I24" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="J24" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="K24" t="s">
         <v>70</v>
@@ -2902,7 +2978,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -2911,19 +2987,19 @@
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="H25" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I25" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="J25" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="K25" t="s">
         <v>70</v>
@@ -2931,7 +3007,7 @@
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -2940,19 +3016,19 @@
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>465</v>
+        <v>425</v>
       </c>
       <c r="H26" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I26" t="s">
-        <v>466</v>
+        <v>426</v>
       </c>
       <c r="J26" t="s">
-        <v>467</v>
+        <v>427</v>
       </c>
       <c r="K26" t="s">
         <v>70</v>
@@ -2960,7 +3036,7 @@
     </row>
     <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -2969,19 +3045,19 @@
         <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="H27" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I27" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="J27" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="K27" t="s">
         <v>70</v>
@@ -2989,7 +3065,7 @@
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -2998,19 +3074,19 @@
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="H28" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I28" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="J28" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="K28" t="s">
         <v>70</v>
@@ -3018,7 +3094,7 @@
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -3027,19 +3103,19 @@
         <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="H29" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I29" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="J29" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="K29" t="s">
         <v>70</v>
@@ -3047,7 +3123,7 @@
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -3056,19 +3132,19 @@
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="H30" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I30" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="J30" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="K30" t="s">
         <v>70</v>
@@ -3076,7 +3152,7 @@
     </row>
     <row r="31" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -3085,19 +3161,19 @@
         <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="F31" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="H31" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I31" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="J31" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="K31" t="s">
         <v>70</v>
@@ -3105,7 +3181,7 @@
     </row>
     <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -3114,27 +3190,27 @@
         <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="H32" t="s">
-        <v>421</v>
+        <v>381</v>
       </c>
       <c r="I32" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="J32" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="K32" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>501</v>
+        <v>525</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -3143,22 +3219,10 @@
         <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>501</v>
+        <v>525</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="H33" t="s">
-        <v>421</v>
-      </c>
-      <c r="I33" t="s">
-        <v>499</v>
-      </c>
-      <c r="J33" t="s">
-        <v>500</v>
-      </c>
-      <c r="K33" t="s">
-        <v>70</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>
@@ -3169,10 +3233,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC91813-AD9F-4B65-8DAD-DE1B79C09543}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3187,7 +3251,7 @@
     <col min="9" max="11" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -3224,13 +3288,16 @@
       <c r="L1" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -3238,8 +3305,29 @@
       <c r="F2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" s="18">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>515</v>
+      </c>
+      <c r="J2" t="s">
+        <v>516</v>
+      </c>
+      <c r="K2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -3253,7 +3341,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -3267,7 +3355,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -3281,7 +3369,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -3294,8 +3382,20 @@
       <c r="F6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>507</v>
+      </c>
+      <c r="J6" t="s">
+        <v>508</v>
+      </c>
+      <c r="K6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>73</v>
       </c>
@@ -3308,8 +3408,20 @@
       <c r="F7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" t="s">
+        <v>509</v>
+      </c>
+      <c r="J7" t="s">
+        <v>510</v>
+      </c>
+      <c r="K7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -3322,8 +3434,20 @@
       <c r="F8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" t="s">
+        <v>511</v>
+      </c>
+      <c r="J8" t="s">
+        <v>512</v>
+      </c>
+      <c r="K8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -3336,8 +3460,20 @@
       <c r="F9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>513</v>
+      </c>
+      <c r="J9" t="s">
+        <v>514</v>
+      </c>
+      <c r="K9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -3351,7 +3487,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -3362,105 +3498,153 @@
         <v>86</v>
       </c>
       <c r="F11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" t="s">
         <v>120</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="H13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" t="s">
+        <v>521</v>
+      </c>
+      <c r="J13" t="s">
+        <v>522</v>
+      </c>
+      <c r="K13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
         <v>122</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="H14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" t="s">
+        <v>523</v>
+      </c>
+      <c r="J14" t="s">
+        <v>524</v>
+      </c>
+      <c r="K14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" t="s">
         <v>124</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="H15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" t="s">
+        <v>517</v>
+      </c>
+      <c r="J15" t="s">
+        <v>518</v>
+      </c>
+      <c r="K15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" t="s">
         <v>126</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" t="s">
-        <v>129</v>
+      <c r="H16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" t="s">
+        <v>519</v>
+      </c>
+      <c r="J16" t="s">
+        <v>520</v>
+      </c>
+      <c r="K16" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3470,10 +3654,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B76D93-F2C0-4CD2-AA8C-AD315425546C}">
-  <dimension ref="A1:N84"/>
+  <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,12 +3669,12 @@
     <col min="6" max="6" width="73.140625" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="12" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -3528,15 +3712,33 @@
         <v>45</v>
       </c>
       <c r="M1" t="s">
-        <v>418</v>
+        <v>378</v>
       </c>
       <c r="N1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+      <c r="O1" t="s">
+        <v>428</v>
+      </c>
+      <c r="P1" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>430</v>
+      </c>
+      <c r="R1" t="s">
+        <v>431</v>
+      </c>
+      <c r="S1" t="s">
+        <v>432</v>
+      </c>
+      <c r="T1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>6</v>
@@ -3551,21 +3753,21 @@
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>6</v>
@@ -3576,25 +3778,25 @@
         <v>15</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J3" t="s">
-        <v>410</v>
+        <v>370</v>
       </c>
       <c r="K3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>6</v>
@@ -3605,25 +3807,25 @@
         <v>22</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I4" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J4" t="s">
-        <v>411</v>
+        <v>371</v>
       </c>
       <c r="K4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>6</v>
@@ -3634,25 +3836,25 @@
         <v>28</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I5" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J5" t="s">
-        <v>412</v>
+        <v>372</v>
       </c>
       <c r="K5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>6</v>
@@ -3663,25 +3865,25 @@
         <v>29</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I6" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J6" t="s">
-        <v>413</v>
+        <v>373</v>
       </c>
       <c r="K6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>6</v>
@@ -3692,25 +3894,25 @@
         <v>30</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I7" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J7" t="s">
-        <v>414</v>
+        <v>374</v>
       </c>
       <c r="K7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>6</v>
@@ -3721,25 +3923,25 @@
         <v>74</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I8" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J8" t="s">
-        <v>415</v>
+        <v>375</v>
       </c>
       <c r="K8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>6</v>
@@ -3750,25 +3952,25 @@
         <v>77</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I9" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J9" t="s">
-        <v>416</v>
+        <v>376</v>
       </c>
       <c r="K9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>6</v>
@@ -3779,25 +3981,25 @@
         <v>80</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" t="s">
+        <v>369</v>
+      </c>
+      <c r="J10" t="s">
+        <v>377</v>
+      </c>
+      <c r="K10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>102</v>
-      </c>
-      <c r="I10" t="s">
-        <v>409</v>
-      </c>
-      <c r="J10" t="s">
-        <v>417</v>
-      </c>
-      <c r="K10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>105</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>6</v>
@@ -3808,25 +4010,25 @@
         <v>83</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I11" t="s">
-        <v>401</v>
+        <v>361</v>
       </c>
       <c r="J11" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="K11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>6</v>
@@ -3837,25 +4039,25 @@
         <v>86</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I12" t="s">
-        <v>393</v>
+        <v>353</v>
       </c>
       <c r="J12" t="s">
-        <v>394</v>
+        <v>354</v>
       </c>
       <c r="K12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>6</v>
@@ -3863,28 +4065,28 @@
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I13" t="s">
-        <v>397</v>
+        <v>357</v>
       </c>
       <c r="J13" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="K13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>6</v>
@@ -3892,28 +4094,28 @@
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I14" t="s">
-        <v>399</v>
+        <v>359</v>
       </c>
       <c r="J14" t="s">
-        <v>400</v>
+        <v>360</v>
       </c>
       <c r="K14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>6</v>
@@ -3921,28 +4123,28 @@
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I15" t="s">
-        <v>395</v>
+        <v>355</v>
       </c>
       <c r="J15" t="s">
-        <v>396</v>
+        <v>356</v>
       </c>
       <c r="K15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>6</v>
@@ -3950,28 +4152,28 @@
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I16" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="J16" t="s">
-        <v>361</v>
+        <v>332</v>
       </c>
       <c r="K16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>6</v>
@@ -3979,28 +4181,28 @@
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I17" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="J17" t="s">
-        <v>362</v>
+        <v>333</v>
       </c>
       <c r="K17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>6</v>
@@ -4008,28 +4210,28 @@
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I18" t="s">
-        <v>405</v>
+        <v>365</v>
       </c>
       <c r="J18" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="K18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>6</v>
@@ -4037,20 +4239,20 @@
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I19" t="s">
-        <v>409</v>
+        <v>369</v>
       </c>
       <c r="J19" t="s">
-        <v>420</v>
+        <v>380</v>
       </c>
       <c r="K19" t="s">
         <v>70</v>
@@ -4065,9 +4267,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>6</v>
@@ -4075,28 +4277,28 @@
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I20" t="s">
-        <v>403</v>
+        <v>363</v>
       </c>
       <c r="J20" t="s">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="K20" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>6</v>
@@ -4104,28 +4306,28 @@
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I21" t="s">
-        <v>373</v>
+        <v>336</v>
       </c>
       <c r="J21" t="s">
-        <v>374</v>
+        <v>337</v>
       </c>
       <c r="K21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>6</v>
@@ -4133,28 +4335,28 @@
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I22" t="s">
-        <v>407</v>
+        <v>367</v>
       </c>
       <c r="J22" t="s">
-        <v>408</v>
+        <v>368</v>
       </c>
       <c r="K22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>6</v>
@@ -4162,28 +4364,40 @@
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I23" t="s">
-        <v>360</v>
+        <v>434</v>
       </c>
       <c r="J23" t="s">
-        <v>363</v>
+        <v>435</v>
       </c>
       <c r="K23" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>132</v>
+      </c>
+      <c r="M23" t="s">
+        <v>132</v>
+      </c>
+      <c r="N23" t="s">
+        <v>132</v>
+      </c>
+      <c r="O23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>6</v>
@@ -4191,28 +4405,28 @@
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I24" t="s">
-        <v>373</v>
+        <v>436</v>
       </c>
       <c r="J24" t="s">
-        <v>375</v>
+        <v>437</v>
       </c>
       <c r="K24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>6</v>
@@ -4220,28 +4434,42 @@
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="G25" s="14"/>
+        <v>287</v>
+      </c>
+      <c r="G25" s="14">
+        <v>4</v>
+      </c>
       <c r="H25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I25" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="J25" t="s">
-        <v>364</v>
+        <v>439</v>
       </c>
       <c r="K25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="L25" t="s">
+        <v>132</v>
+      </c>
+      <c r="M25" t="s">
+        <v>132</v>
+      </c>
+      <c r="N25" t="s">
+        <v>132</v>
+      </c>
+      <c r="O25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>6</v>
@@ -4249,28 +4477,28 @@
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I26" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="J26" t="s">
-        <v>365</v>
+        <v>334</v>
       </c>
       <c r="K26" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>6</v>
@@ -4278,28 +4506,42 @@
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="G27" s="14"/>
+        <v>281</v>
+      </c>
+      <c r="G27" s="14">
+        <v>4</v>
+      </c>
       <c r="H27" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I27" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="J27" t="s">
-        <v>366</v>
+        <v>440</v>
       </c>
       <c r="K27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="L27" t="s">
+        <v>132</v>
+      </c>
+      <c r="M27" t="s">
+        <v>132</v>
+      </c>
+      <c r="N27" t="s">
+        <v>132</v>
+      </c>
+      <c r="O27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>6</v>
@@ -4307,28 +4549,28 @@
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="G28" s="14"/>
       <c r="H28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I28" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="J28" t="s">
-        <v>367</v>
+        <v>441</v>
       </c>
       <c r="K28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>6</v>
@@ -4336,28 +4578,42 @@
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>300</v>
-      </c>
-      <c r="G29" s="14"/>
+        <v>283</v>
+      </c>
+      <c r="G29" s="14">
+        <v>4</v>
+      </c>
       <c r="H29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I29" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="J29" t="s">
-        <v>368</v>
+        <v>442</v>
       </c>
       <c r="K29" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M29" t="s">
+        <v>132</v>
+      </c>
+      <c r="N29" t="s">
+        <v>132</v>
+      </c>
+      <c r="O29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>6</v>
@@ -4365,28 +4621,28 @@
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>305</v>
+        <v>464</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I30" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="J30" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
       <c r="K30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>6</v>
@@ -4394,28 +4650,42 @@
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="G31" s="14"/>
+        <v>288</v>
+      </c>
+      <c r="G31" s="14">
+        <v>4</v>
+      </c>
       <c r="H31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I31" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="J31" t="s">
-        <v>370</v>
+        <v>443</v>
       </c>
       <c r="K31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="L31" t="s">
+        <v>132</v>
+      </c>
+      <c r="M31" t="s">
+        <v>132</v>
+      </c>
+      <c r="N31" t="s">
+        <v>132</v>
+      </c>
+      <c r="O31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>6</v>
@@ -4423,28 +4693,28 @@
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I32" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="J32" t="s">
-        <v>371</v>
+        <v>444</v>
       </c>
       <c r="K32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>6</v>
@@ -4452,28 +4722,42 @@
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>308</v>
-      </c>
-      <c r="G33" s="14"/>
+        <v>290</v>
+      </c>
+      <c r="G33" s="14">
+        <v>4</v>
+      </c>
       <c r="H33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I33" t="s">
-        <v>360</v>
+        <v>438</v>
       </c>
       <c r="J33" t="s">
-        <v>372</v>
+        <v>445</v>
       </c>
       <c r="K33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="L33" t="s">
+        <v>132</v>
+      </c>
+      <c r="M33" t="s">
+        <v>132</v>
+      </c>
+      <c r="N33" t="s">
+        <v>132</v>
+      </c>
+      <c r="O33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>6</v>
@@ -4481,28 +4765,28 @@
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>309</v>
+        <v>465</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I34" t="s">
-        <v>373</v>
+        <v>336</v>
       </c>
       <c r="J34" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="K34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>6</v>
@@ -4510,28 +4794,37 @@
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I35" t="s">
-        <v>377</v>
+        <v>446</v>
       </c>
       <c r="J35" t="s">
-        <v>378</v>
+        <v>447</v>
       </c>
       <c r="K35" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>132</v>
+      </c>
+      <c r="M35" t="s">
+        <v>132</v>
+      </c>
+      <c r="N35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>6</v>
@@ -4539,28 +4832,57 @@
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>311</v>
-      </c>
-      <c r="G36" s="14"/>
+        <v>292</v>
+      </c>
+      <c r="G36" s="14">
+        <v>10</v>
+      </c>
       <c r="H36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I36" t="s">
-        <v>377</v>
+        <v>448</v>
       </c>
       <c r="J36" t="s">
-        <v>379</v>
+        <v>449</v>
       </c>
       <c r="K36" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>70</v>
+      </c>
+      <c r="M36" t="s">
+        <v>70</v>
+      </c>
+      <c r="N36" t="s">
+        <v>70</v>
+      </c>
+      <c r="O36" t="s">
+        <v>132</v>
+      </c>
+      <c r="P36" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>70</v>
+      </c>
+      <c r="R36" t="s">
+        <v>132</v>
+      </c>
+      <c r="S36" t="s">
+        <v>132</v>
+      </c>
+      <c r="T36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>6</v>
@@ -4568,28 +4890,28 @@
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="G37" s="14"/>
       <c r="H37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I37" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
       <c r="J37" t="s">
-        <v>380</v>
+        <v>340</v>
       </c>
       <c r="K37" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>6</v>
@@ -4597,28 +4919,28 @@
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="F38" s="17" t="s">
-        <v>314</v>
+        <v>203</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>295</v>
       </c>
       <c r="G38" s="14"/>
       <c r="H38" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I38" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="J38" t="s">
-        <v>382</v>
+        <v>342</v>
       </c>
       <c r="K38" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>6</v>
@@ -4626,28 +4948,28 @@
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>313</v>
+        <v>204</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>294</v>
       </c>
       <c r="G39" s="14"/>
       <c r="H39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I39" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="J39" t="s">
-        <v>383</v>
+        <v>343</v>
       </c>
       <c r="K39" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>6</v>
@@ -4655,28 +4977,28 @@
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>315</v>
+        <v>205</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>296</v>
       </c>
       <c r="G40" s="14"/>
       <c r="H40" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I40" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="J40" t="s">
-        <v>384</v>
+        <v>344</v>
       </c>
       <c r="K40" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>6</v>
@@ -4684,28 +5006,28 @@
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="F41" s="17" t="s">
-        <v>316</v>
+        <v>206</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>297</v>
       </c>
       <c r="G41" s="14"/>
       <c r="H41" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I41" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="J41" t="s">
-        <v>385</v>
+        <v>345</v>
       </c>
       <c r="K41" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>6</v>
@@ -4713,28 +5035,28 @@
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="F42" s="17" t="s">
-        <v>317</v>
+        <v>207</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>298</v>
       </c>
       <c r="G42" s="14"/>
       <c r="H42" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I42" t="s">
-        <v>381</v>
+        <v>341</v>
       </c>
       <c r="J42" t="s">
-        <v>386</v>
+        <v>346</v>
       </c>
       <c r="K42" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>6</v>
@@ -4742,28 +5064,28 @@
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="F43" s="18" t="s">
-        <v>318</v>
+        <v>208</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>299</v>
       </c>
       <c r="G43" s="14"/>
       <c r="H43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I43" t="s">
-        <v>387</v>
+        <v>347</v>
       </c>
       <c r="J43" t="s">
-        <v>388</v>
+        <v>348</v>
       </c>
       <c r="K43" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>6</v>
@@ -4771,28 +5093,28 @@
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>319</v>
+        <v>209</v>
+      </c>
+      <c r="F44" s="16" t="s">
+        <v>300</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I44" t="s">
-        <v>389</v>
+        <v>349</v>
       </c>
       <c r="J44" t="s">
-        <v>390</v>
+        <v>350</v>
       </c>
       <c r="K44" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>6</v>
@@ -4800,28 +5122,28 @@
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>320</v>
+        <v>210</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>301</v>
       </c>
       <c r="G45" s="14"/>
       <c r="H45" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I45" t="s">
-        <v>389</v>
+        <v>349</v>
       </c>
       <c r="J45" t="s">
-        <v>391</v>
+        <v>351</v>
       </c>
       <c r="K45" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>6</v>
@@ -4829,28 +5151,28 @@
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="G46" s="14"/>
       <c r="H46" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I46" t="s">
-        <v>389</v>
+        <v>349</v>
       </c>
       <c r="J46" t="s">
-        <v>392</v>
+        <v>352</v>
       </c>
       <c r="K46" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>6</v>
@@ -4858,10 +5180,10 @@
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="G47" s="14"/>
       <c r="H47" s="14"/>
@@ -4869,30 +5191,38 @@
       <c r="J47" s="14"/>
       <c r="K47" s="14"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
+      <c r="H48" t="s">
+        <v>99</v>
+      </c>
+      <c r="I48" t="s">
+        <v>450</v>
+      </c>
+      <c r="J48" t="s">
+        <v>451</v>
+      </c>
+      <c r="K48" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>6</v>
@@ -4900,10 +5230,10 @@
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
@@ -4913,7 +5243,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>6</v>
@@ -4921,10 +5251,10 @@
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>325</v>
+        <v>306</v>
       </c>
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
@@ -4934,7 +5264,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>6</v>
@@ -4942,10 +5272,10 @@
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
@@ -4955,7 +5285,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B52" s="14" t="s">
         <v>6</v>
@@ -4963,10 +5293,10 @@
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>278</v>
+        <v>216</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>261</v>
       </c>
       <c r="G52" s="14"/>
       <c r="H52" s="14"/>
@@ -4976,18 +5306,18 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
-      <c r="E53" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>279</v>
+      <c r="E53" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>262</v>
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
@@ -4997,18 +5327,18 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
-      <c r="E54" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>280</v>
+      <c r="E54" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>263</v>
       </c>
       <c r="G54" s="14"/>
       <c r="H54" s="14"/>
@@ -5018,28 +5348,28 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
-      <c r="E55" s="15" t="s">
-        <v>187</v>
+      <c r="E55" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="G55" s="14"/>
       <c r="H55" s="14" t="s">
         <v>69</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J55" s="14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K55" s="14" t="s">
         <v>70</v>
@@ -5047,28 +5377,28 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
-      <c r="E56" s="15" t="s">
-        <v>184</v>
+      <c r="E56" s="14" t="s">
+        <v>181</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="G56" s="14"/>
       <c r="H56" s="14" t="s">
         <v>69</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J56" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K56" s="14" t="s">
         <v>70</v>
@@ -5076,28 +5406,28 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
-      <c r="E57" s="15" t="s">
-        <v>185</v>
+      <c r="E57" s="14" t="s">
+        <v>182</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="G57" s="14"/>
       <c r="H57" s="14" t="s">
         <v>69</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J57" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K57" s="14" t="s">
         <v>70</v>
@@ -5105,18 +5435,18 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
-      <c r="E58" s="15" t="s">
-        <v>221</v>
+      <c r="E58" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="G58" s="14"/>
       <c r="H58" s="14"/>
@@ -5126,18 +5456,18 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
-      <c r="E59" s="15" t="s">
-        <v>223</v>
+      <c r="E59" s="14" t="s">
+        <v>220</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
@@ -5147,18 +5477,18 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B60" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
-      <c r="E60" s="15" t="s">
-        <v>225</v>
+      <c r="E60" s="14" t="s">
+        <v>222</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="G60" s="14"/>
       <c r="H60" s="14"/>
@@ -5168,123 +5498,163 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B61" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
-      <c r="E61" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>333</v>
+      <c r="E61" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>314</v>
       </c>
       <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
+      <c r="H61" t="s">
+        <v>69</v>
+      </c>
+      <c r="I61" t="s">
+        <v>454</v>
+      </c>
+      <c r="J61" t="s">
+        <v>455</v>
+      </c>
+      <c r="K61" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B62" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
-      <c r="E62" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>334</v>
+      <c r="E62" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>315</v>
       </c>
       <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
+      <c r="H62" t="s">
+        <v>69</v>
+      </c>
+      <c r="I62" t="s">
+        <v>454</v>
+      </c>
+      <c r="J62" t="s">
+        <v>456</v>
+      </c>
+      <c r="K62" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B63" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
-      <c r="E63" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="F63" s="17" t="s">
-        <v>335</v>
+      <c r="E63" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
+      <c r="H63" t="s">
+        <v>69</v>
+      </c>
+      <c r="I63" t="s">
+        <v>457</v>
+      </c>
+      <c r="J63" t="s">
+        <v>458</v>
+      </c>
+      <c r="K63" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B64" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
-      <c r="E64" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="F64" s="17" t="s">
-        <v>336</v>
+      <c r="E64" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>453</v>
       </c>
       <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
+      <c r="H64" t="s">
+        <v>69</v>
+      </c>
+      <c r="I64" t="s">
+        <v>461</v>
+      </c>
+      <c r="J64" t="s">
+        <v>462</v>
+      </c>
+      <c r="K64" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
-      <c r="E65" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="F65" s="17" t="s">
-        <v>337</v>
+      <c r="E65" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>452</v>
       </c>
       <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
+      <c r="H65" t="s">
+        <v>69</v>
+      </c>
+      <c r="I65" t="s">
+        <v>459</v>
+      </c>
+      <c r="J65" t="s">
+        <v>460</v>
+      </c>
+      <c r="K65" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B66" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
-      <c r="E66" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="F66" s="17" t="s">
-        <v>338</v>
+      <c r="E66" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>317</v>
       </c>
       <c r="G66" s="14"/>
       <c r="H66" s="14"/>
@@ -5294,49 +5664,57 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B67" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
-      <c r="E67" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="F67" s="17" t="s">
-        <v>339</v>
+      <c r="E67" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>318</v>
       </c>
       <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
+      <c r="H67" t="s">
+        <v>69</v>
+      </c>
+      <c r="I67" t="s">
+        <v>257</v>
+      </c>
+      <c r="J67" t="s">
+        <v>258</v>
+      </c>
+      <c r="K67" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B68" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
-      <c r="E68" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="F68" s="17" t="s">
-        <v>340</v>
+      <c r="E68" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>319</v>
       </c>
       <c r="G68" s="14"/>
       <c r="H68" t="s">
         <v>69</v>
       </c>
       <c r="I68" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="J68" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="K68" t="s">
         <v>70</v>
@@ -5344,68 +5722,68 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B69" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
-      <c r="E69" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="F69" s="17" t="s">
-        <v>341</v>
+      <c r="E69" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="G69" s="14"/>
-      <c r="H69" t="s">
-        <v>69</v>
-      </c>
-      <c r="I69" t="s">
-        <v>276</v>
-      </c>
-      <c r="J69" t="s">
-        <v>277</v>
-      </c>
-      <c r="K69" t="s">
-        <v>70</v>
-      </c>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
-      <c r="E70" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="F70" s="17" t="s">
-        <v>342</v>
+      <c r="E70" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
+      <c r="H70" t="s">
+        <v>69</v>
+      </c>
+      <c r="I70" t="s">
+        <v>466</v>
+      </c>
+      <c r="J70" t="s">
+        <v>467</v>
+      </c>
+      <c r="K70" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B71" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
-      <c r="E71" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="F71" s="17" t="s">
-        <v>343</v>
+      <c r="E71" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>463</v>
       </c>
       <c r="G71" s="14"/>
       <c r="H71" s="14"/>
@@ -5415,39 +5793,47 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B72" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
-      <c r="E72" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="F72" s="17" t="s">
-        <v>344</v>
+      <c r="E72" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="F72" s="15" t="s">
+        <v>322</v>
       </c>
       <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-      <c r="K72" s="14"/>
+      <c r="H72" t="s">
+        <v>69</v>
+      </c>
+      <c r="I72" t="s">
+        <v>466</v>
+      </c>
+      <c r="J72" t="s">
+        <v>468</v>
+      </c>
+      <c r="K72" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B73" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
-      <c r="E73" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="F73" s="17" t="s">
-        <v>345</v>
+      <c r="E73" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>323</v>
       </c>
       <c r="G73" s="14"/>
       <c r="H73" s="14"/>
@@ -5457,39 +5843,47 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
-      <c r="E74" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="F74" s="17" t="s">
-        <v>346</v>
+      <c r="E74" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="F74" s="15" t="s">
+        <v>324</v>
       </c>
       <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14"/>
+      <c r="H74" t="s">
+        <v>69</v>
+      </c>
+      <c r="I74" t="s">
+        <v>504</v>
+      </c>
+      <c r="J74" t="s">
+        <v>505</v>
+      </c>
+      <c r="K74" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B75" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
-      <c r="E75" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>347</v>
+      <c r="E75" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="F75" s="15" t="s">
+        <v>326</v>
       </c>
       <c r="G75" s="14"/>
       <c r="H75" s="14"/>
@@ -5499,18 +5893,18 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B76" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
-      <c r="E76" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>348</v>
+      <c r="E76" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="G76" s="14"/>
       <c r="H76" s="14"/>
@@ -5520,171 +5914,24 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B77" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C77" s="14"/>
       <c r="D77" s="14"/>
-      <c r="E77" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="F77" s="17" t="s">
-        <v>349</v>
+      <c r="E77" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>327</v>
       </c>
       <c r="G77" s="14"/>
       <c r="H77" s="14"/>
       <c r="I77" s="14"/>
       <c r="J77" s="14"/>
       <c r="K77" s="14"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
-      <c r="J78" s="14"/>
-      <c r="K78" s="14"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="B79" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>351</v>
-      </c>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
-      <c r="I79" s="14"/>
-      <c r="J79" s="14"/>
-      <c r="K79" s="14"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="B80" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="F80" s="17" t="s">
-        <v>352</v>
-      </c>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
-      <c r="J80" s="14"/>
-      <c r="K80" s="14"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="B81" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="F81" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
-      <c r="K81" s="14"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="B82" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="F82" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
-      <c r="I82" s="14"/>
-      <c r="J82" s="14"/>
-      <c r="K82" s="14"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="F83" s="17" t="s">
-        <v>355</v>
-      </c>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
-      <c r="J83" s="14"/>
-      <c r="K83" s="14"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="15" t="s">
-        <v>273</v>
-      </c>
-      <c r="F84" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="14"/>
-      <c r="K84" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
New changes of CC
</commit_message>
<xml_diff>
--- a/src/main/resources/testdesign/testcontroller/master.xlsx
+++ b/src/main/resources/testdesign/testcontroller/master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiservcorp-my.sharepoint.com/personal/moksha_mukh_fiserv_com/Documents/Desktop/Republic UAT/TestAutomation/git/workspace/Test_Automation/src/main/resources/testdesign/testcontroller/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New_FrameWork\Git\Workspace\Test_Automation\src\main\resources\testdesign\testcontroller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{DAF2207D-6EEF-4B6A-A45F-E4DA9721D19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D6BFA59-14EE-48C2-8F31-DDFD2672A36B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2C2102-CE52-4E48-A4F3-B738A962DAE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="533">
   <si>
     <t>Application_Name</t>
   </si>
@@ -1188,58 +1187,16 @@
     <t>sthangapalam</t>
   </si>
   <si>
-    <t>'2021/12/23 16:53:46</t>
-  </si>
-  <si>
-    <t>'2021/12/23 16:56:12</t>
-  </si>
-  <si>
-    <t>'2021/12/23 21:35:20</t>
-  </si>
-  <si>
-    <t>'2021/12/23 21:42:51</t>
-  </si>
-  <si>
-    <t>'2021/12/23 21:48:42</t>
-  </si>
-  <si>
     <t>'2021/12/22 16:56:10</t>
   </si>
   <si>
     <t>'2021/12/22 17:15:05</t>
   </si>
   <si>
-    <t>'2021/12/23 19:31:45</t>
-  </si>
-  <si>
-    <t>'2021/12/23 19:39:36</t>
-  </si>
-  <si>
-    <t>'2021/12/23 21:58:14</t>
-  </si>
-  <si>
-    <t>'2021/12/24 12:27:18</t>
-  </si>
-  <si>
-    <t>'2021/12/24 12:39:16</t>
-  </si>
-  <si>
-    <t>'2022/01/03 12:58:15</t>
-  </si>
-  <si>
-    <t>'2022/01/03 13:01:06</t>
-  </si>
-  <si>
     <t>'2022/01/03 17:22:57</t>
   </si>
   <si>
     <t>'2022/01/03 17:29:38</t>
-  </si>
-  <si>
-    <t>'2022/01/03 17:42:48</t>
-  </si>
-  <si>
-    <t>'2022/01/03 17:48:05</t>
   </si>
   <si>
     <t>CC_CORP_TC012</t>
@@ -1641,6 +1598,68 @@
   </si>
   <si>
     <t>Create a wire transfer template (free form)and search it</t>
+  </si>
+  <si>
+    <t>'2022/01/21 12:56:00</t>
+  </si>
+  <si>
+    <t>'2022/01/21 13:44:26</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC039</t>
+  </si>
+  <si>
+    <t>Initiate Ach Payment(Zero Payment) using free form- Approval
+if Existing template , do a payment activity
+elseCreate batch template, use that template and do payments</t>
+  </si>
+  <si>
+    <t>'2022/01/24 15:24:40</t>
+  </si>
+  <si>
+    <t>'2022/01/24 15:27:08</t>
+  </si>
+  <si>
+    <t>'2022/01/24 16:02:28</t>
+  </si>
+  <si>
+    <t>'2022/01/24 16:09:57</t>
+  </si>
+  <si>
+    <t>'2022/01/24 18:12:39</t>
+  </si>
+  <si>
+    <t>'2022/01/24 19:00:28</t>
+  </si>
+  <si>
+    <t>'2022/01/24 19:23:16</t>
+  </si>
+  <si>
+    <t>'2022/01/24 19:57:47</t>
+  </si>
+  <si>
+    <t>'2022/01/24 20:43:58</t>
+  </si>
+  <si>
+    <t>'2022/01/24 20:46:26</t>
+  </si>
+  <si>
+    <t>'2022/01/24 21:03:05</t>
+  </si>
+  <si>
+    <t>'2022/01/24 21:07:13</t>
+  </si>
+  <si>
+    <t>'2022/01/25 11:25:10</t>
+  </si>
+  <si>
+    <t>'2022/01/25 11:31:23</t>
+  </si>
+  <si>
+    <t>CC_CORP_TC032</t>
+  </si>
+  <si>
+    <t>Initiate Wire transfer Payment  using wire  select free form- Reject, Initiatior- cancel</t>
   </si>
 </sst>
 </file>
@@ -2185,7 +2204,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,13 +2234,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2240,7 +2259,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -2276,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5698D2-2A68-44BF-B3E0-84682E6FAE93}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="79" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="79" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,10 +2430,10 @@
         <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="J4" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="K4" t="s">
         <v>70</v>
@@ -2440,10 +2459,10 @@
         <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="J5" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="K5" t="s">
         <v>70</v>
@@ -2486,10 +2505,10 @@
         <v>381</v>
       </c>
       <c r="I7" t="s">
-        <v>382</v>
+        <v>517</v>
       </c>
       <c r="J7" t="s">
-        <v>383</v>
+        <v>518</v>
       </c>
       <c r="K7" t="s">
         <v>70</v>
@@ -2515,13 +2534,13 @@
         <v>381</v>
       </c>
       <c r="I8" t="s">
-        <v>384</v>
+        <v>519</v>
       </c>
       <c r="J8" t="s">
-        <v>385</v>
+        <v>520</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2544,10 +2563,10 @@
         <v>381</v>
       </c>
       <c r="I9" t="s">
-        <v>384</v>
+        <v>521</v>
       </c>
       <c r="J9" t="s">
-        <v>386</v>
+        <v>522</v>
       </c>
       <c r="K9" t="s">
         <v>70</v>
@@ -2573,10 +2592,10 @@
         <v>381</v>
       </c>
       <c r="I10" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="J10" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="K10" t="s">
         <v>70</v>
@@ -2602,10 +2621,10 @@
         <v>381</v>
       </c>
       <c r="I11" t="s">
-        <v>389</v>
+        <v>523</v>
       </c>
       <c r="J11" t="s">
-        <v>390</v>
+        <v>524</v>
       </c>
       <c r="K11" t="s">
         <v>70</v>
@@ -2631,13 +2650,13 @@
         <v>381</v>
       </c>
       <c r="I12" t="s">
-        <v>384</v>
+        <v>529</v>
       </c>
       <c r="J12" t="s">
-        <v>391</v>
+        <v>530</v>
       </c>
       <c r="K12" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2660,10 +2679,10 @@
         <v>381</v>
       </c>
       <c r="I13" t="s">
-        <v>392</v>
+        <v>525</v>
       </c>
       <c r="J13" t="s">
-        <v>393</v>
+        <v>526</v>
       </c>
       <c r="K13" t="s">
         <v>70</v>
@@ -2689,10 +2708,10 @@
         <v>381</v>
       </c>
       <c r="I14" t="s">
-        <v>394</v>
+        <v>527</v>
       </c>
       <c r="J14" t="s">
-        <v>395</v>
+        <v>528</v>
       </c>
       <c r="K14" t="s">
         <v>70</v>
@@ -2718,10 +2737,10 @@
         <v>381</v>
       </c>
       <c r="I15" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="J15" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="K15" t="s">
         <v>70</v>
@@ -2732,7 +2751,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -2747,13 +2766,13 @@
         <v>381</v>
       </c>
       <c r="I16" t="s">
-        <v>398</v>
+        <v>513</v>
       </c>
       <c r="J16" t="s">
-        <v>399</v>
+        <v>514</v>
       </c>
       <c r="K16" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2775,7 +2794,7 @@
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -2784,19 +2803,19 @@
         <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="H18" t="s">
         <v>381</v>
       </c>
       <c r="I18" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="J18" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="K18" t="s">
         <v>70</v>
@@ -2804,7 +2823,7 @@
     </row>
     <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -2813,19 +2832,19 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="H19" t="s">
         <v>381</v>
       </c>
       <c r="I19" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="J19" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="K19" t="s">
         <v>70</v>
@@ -2833,7 +2852,7 @@
     </row>
     <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -2842,19 +2861,19 @@
         <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="H20" t="s">
         <v>381</v>
       </c>
       <c r="I20" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="J20" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="K20" t="s">
         <v>70</v>
@@ -2862,7 +2881,7 @@
     </row>
     <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -2871,19 +2890,19 @@
         <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="H21" t="s">
         <v>381</v>
       </c>
       <c r="I21" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="J21" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="K21" t="s">
         <v>70</v>
@@ -2891,7 +2910,7 @@
     </row>
     <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -2900,19 +2919,19 @@
         <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="H22" t="s">
         <v>381</v>
       </c>
       <c r="I22" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="J22" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="K22" t="s">
         <v>70</v>
@@ -2920,7 +2939,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -2929,19 +2948,19 @@
         <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="H23" t="s">
         <v>381</v>
       </c>
       <c r="I23" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="J23" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="K23" t="s">
         <v>70</v>
@@ -2949,7 +2968,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -2958,19 +2977,19 @@
         <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="H24" t="s">
         <v>381</v>
       </c>
       <c r="I24" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="J24" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="K24" t="s">
         <v>70</v>
@@ -2978,7 +2997,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -2987,19 +3006,19 @@
         <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="H25" t="s">
         <v>381</v>
       </c>
       <c r="I25" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="J25" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="K25" t="s">
         <v>70</v>
@@ -3007,7 +3026,7 @@
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -3016,19 +3035,19 @@
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="H26" t="s">
         <v>381</v>
       </c>
       <c r="I26" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="J26" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="K26" t="s">
         <v>70</v>
@@ -3036,7 +3055,7 @@
     </row>
     <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -3045,19 +3064,19 @@
         <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="H27" t="s">
         <v>381</v>
       </c>
       <c r="I27" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="J27" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="K27" t="s">
         <v>70</v>
@@ -3065,7 +3084,7 @@
     </row>
     <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -3074,19 +3093,19 @@
         <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="H28" t="s">
         <v>381</v>
       </c>
       <c r="I28" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="J28" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="K28" t="s">
         <v>70</v>
@@ -3094,7 +3113,7 @@
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -3103,19 +3122,19 @@
         <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="H29" t="s">
         <v>381</v>
       </c>
       <c r="I29" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="J29" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="K29" t="s">
         <v>70</v>
@@ -3123,7 +3142,7 @@
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -3132,19 +3151,19 @@
         <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="H30" t="s">
         <v>381</v>
       </c>
       <c r="I30" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="J30" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="K30" t="s">
         <v>70</v>
@@ -3152,7 +3171,7 @@
     </row>
     <row r="31" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -3161,19 +3180,19 @@
         <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="F31" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="H31" t="s">
         <v>381</v>
       </c>
       <c r="I31" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="J31" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="K31" t="s">
         <v>70</v>
@@ -3181,7 +3200,7 @@
     </row>
     <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -3190,19 +3209,19 @@
         <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="H32" t="s">
         <v>381</v>
       </c>
       <c r="I32" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="J32" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="K32" t="s">
         <v>70</v>
@@ -3210,7 +3229,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -3219,10 +3238,44 @@
         <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>526</v>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>531</v>
+      </c>
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>531</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>515</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" t="s">
+        <v>515</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -3312,10 +3365,10 @@
         <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="J2" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="K2" t="s">
         <v>132</v>
@@ -3386,10 +3439,10 @@
         <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="J6" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="K6" t="s">
         <v>132</v>
@@ -3412,10 +3465,10 @@
         <v>69</v>
       </c>
       <c r="I7" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="J7" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="K7" t="s">
         <v>132</v>
@@ -3438,10 +3491,10 @@
         <v>69</v>
       </c>
       <c r="I8" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="J8" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="K8" t="s">
         <v>132</v>
@@ -3464,10 +3517,10 @@
         <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="J9" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="K9" t="s">
         <v>70</v>
@@ -3532,10 +3585,10 @@
         <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="J13" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="K13" t="s">
         <v>132</v>
@@ -3558,10 +3611,10 @@
         <v>69</v>
       </c>
       <c r="I14" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="J14" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="K14" t="s">
         <v>70</v>
@@ -3584,10 +3637,10 @@
         <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="J15" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="K15" t="s">
         <v>132</v>
@@ -3610,10 +3663,10 @@
         <v>69</v>
       </c>
       <c r="I16" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
       <c r="J16" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="K16" t="s">
         <v>70</v>
@@ -3718,22 +3771,22 @@
         <v>379</v>
       </c>
       <c r="O1" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="P1" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="Q1" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="R1" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="S1" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="T1" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -4374,10 +4427,10 @@
         <v>99</v>
       </c>
       <c r="I23" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="J23" t="s">
-        <v>435</v>
+        <v>421</v>
       </c>
       <c r="K23" t="s">
         <v>70</v>
@@ -4415,10 +4468,10 @@
         <v>99</v>
       </c>
       <c r="I24" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="J24" t="s">
-        <v>437</v>
+        <v>423</v>
       </c>
       <c r="K24" t="s">
         <v>70</v>
@@ -4446,10 +4499,10 @@
         <v>99</v>
       </c>
       <c r="I25" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="J25" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="K25" t="s">
         <v>132</v>
@@ -4518,10 +4571,10 @@
         <v>99</v>
       </c>
       <c r="I27" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="J27" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
       <c r="K27" t="s">
         <v>132</v>
@@ -4559,10 +4612,10 @@
         <v>99</v>
       </c>
       <c r="I28" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="J28" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="K28" t="s">
         <v>132</v>
@@ -4590,10 +4643,10 @@
         <v>99</v>
       </c>
       <c r="I29" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="J29" t="s">
-        <v>442</v>
+        <v>428</v>
       </c>
       <c r="K29" t="s">
         <v>70</v>
@@ -4624,7 +4677,7 @@
         <v>156</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" t="s">
@@ -4662,10 +4715,10 @@
         <v>99</v>
       </c>
       <c r="I31" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="J31" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
       <c r="K31" t="s">
         <v>132</v>
@@ -4703,10 +4756,10 @@
         <v>99</v>
       </c>
       <c r="I32" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="J32" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
       <c r="K32" t="s">
         <v>132</v>
@@ -4734,10 +4787,10 @@
         <v>99</v>
       </c>
       <c r="I33" t="s">
-        <v>438</v>
+        <v>424</v>
       </c>
       <c r="J33" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
       <c r="K33" t="s">
         <v>132</v>
@@ -4768,7 +4821,7 @@
         <v>164</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" t="s">
@@ -4804,10 +4857,10 @@
         <v>99</v>
       </c>
       <c r="I35" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="J35" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="K35" t="s">
         <v>70</v>
@@ -4844,10 +4897,10 @@
         <v>99</v>
       </c>
       <c r="I36" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
       <c r="J36" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
       <c r="K36" t="s">
         <v>70</v>
@@ -5211,10 +5264,10 @@
         <v>99</v>
       </c>
       <c r="I48" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
       <c r="J48" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
       <c r="K48" t="s">
         <v>70</v>
@@ -5516,10 +5569,10 @@
         <v>69</v>
       </c>
       <c r="I61" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="J61" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
       <c r="K61" t="s">
         <v>70</v>
@@ -5545,10 +5598,10 @@
         <v>69</v>
       </c>
       <c r="I62" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="J62" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
       <c r="K62" t="s">
         <v>70</v>
@@ -5574,10 +5627,10 @@
         <v>69</v>
       </c>
       <c r="I63" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="J63" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="K63" t="s">
         <v>70</v>
@@ -5596,17 +5649,17 @@
         <v>230</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
       <c r="G64" s="14"/>
       <c r="H64" t="s">
         <v>69</v>
       </c>
       <c r="I64" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="J64" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="K64" t="s">
         <v>70</v>
@@ -5625,17 +5678,17 @@
         <v>232</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
       <c r="G65" s="14"/>
       <c r="H65" t="s">
         <v>69</v>
       </c>
       <c r="I65" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="J65" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="K65" t="s">
         <v>70</v>
@@ -5761,10 +5814,10 @@
         <v>69</v>
       </c>
       <c r="I70" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="J70" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="K70" t="s">
         <v>70</v>
@@ -5783,7 +5836,7 @@
         <v>244</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="G71" s="14"/>
       <c r="H71" s="14"/>
@@ -5811,10 +5864,10 @@
         <v>69</v>
       </c>
       <c r="I72" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="J72" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="K72" t="s">
         <v>70</v>
@@ -5861,10 +5914,10 @@
         <v>69</v>
       </c>
       <c r="I74" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="J74" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="K74" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
Update new changes on EPP
</commit_message>
<xml_diff>
--- a/src/main/resources/testdesign/testcontroller/master.xlsx
+++ b/src/main/resources/testdesign/testcontroller/master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiservcorp-my.sharepoint.com/personal/moksha_mukh_fiserv_com/Documents/Desktop/Republic UAT/TestAutomation/git/workspace/Test_Automation/src/main/resources/testdesign/testcontroller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{A32160D8-A2FB-4473-A29A-2446DBE517AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02728C62-4314-41CD-922E-2346080B5AD7}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{A32160D8-A2FB-4473-A29A-2446DBE517AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{037991BE-9395-431E-9AE5-8AE00747D25E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="598">
   <si>
     <t>Application_Name</t>
   </si>
@@ -1820,25 +1820,40 @@
     <t>Verify that an Outgoing transaction failed in GFC can be cancelled successfully</t>
   </si>
   <si>
-    <t>'2022/02/03 21:33:30</t>
-  </si>
-  <si>
-    <t>'2022/02/03 21:37:11</t>
-  </si>
-  <si>
     <t>EPP_TC019</t>
   </si>
   <si>
     <t>Verify that an Outgoing transaction failed in GFC can be release successfully</t>
   </si>
   <si>
+    <t>'2022/02/03 21:54:01</t>
+  </si>
+  <si>
+    <t>'2022/02/03 22:11:29</t>
+  </si>
+  <si>
+    <t>EPP_TC021</t>
+  </si>
+  <si>
+    <t>'2022/02/04 23:57:53</t>
+  </si>
+  <si>
+    <t>'2022/02/05 00:09:37</t>
+  </si>
+  <si>
+    <t>EPP_TC020</t>
+  </si>
+  <si>
+    <t>Verify that an Outgoing transaction failed in GFC can be repair and approved successfully</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>'2022/02/03 21:54:01</t>
-  </si>
-  <si>
-    <t>'2022/02/03 22:11:29</t>
+    <t>'2022/02/05 00:43:01</t>
+  </si>
+  <si>
+    <t>'2022/02/05 00:52:20</t>
   </si>
 </sst>
 </file>
@@ -1918,7 +1933,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2068,12 +2083,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2103,7 +2131,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2127,9 +2154,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3462,10 +3497,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC91813-AD9F-4B65-8DAD-DE1B79C09543}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3481,28 +3516,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="22" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="8" t="s">
@@ -3525,19 +3560,21 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="26"/>
       <c r="H2" t="s">
         <v>69</v>
       </c>
@@ -3552,60 +3589,72 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B3" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>55</v>
       </c>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B4" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>57</v>
       </c>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B5" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="10" t="s">
         <v>59</v>
       </c>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B6" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="G6" s="25"/>
       <c r="H6" t="s">
         <v>69</v>
       </c>
@@ -3620,18 +3669,21 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B7" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>75</v>
       </c>
+      <c r="G7" s="25"/>
       <c r="H7" t="s">
         <v>69</v>
       </c>
@@ -3646,18 +3698,21 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B8" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>78</v>
       </c>
+      <c r="G8" s="25"/>
       <c r="H8" t="s">
         <v>69</v>
       </c>
@@ -3672,18 +3727,21 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="B9" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>81</v>
       </c>
+      <c r="G9" s="25"/>
       <c r="H9" t="s">
         <v>69</v>
       </c>
@@ -3698,18 +3756,21 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B10" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="10" t="s">
         <v>84</v>
       </c>
+      <c r="G10" s="25"/>
       <c r="H10" t="s">
         <v>69</v>
       </c>
@@ -3724,18 +3785,21 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="B11" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="10" t="s">
         <v>116</v>
       </c>
+      <c r="G11" s="25"/>
       <c r="H11" t="s">
         <v>69</v>
       </c>
@@ -3750,18 +3814,21 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="B12" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>118</v>
       </c>
+      <c r="G12" s="25"/>
       <c r="H12" t="s">
         <v>69</v>
       </c>
@@ -3776,18 +3843,21 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B13" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="10" t="s">
         <v>120</v>
       </c>
+      <c r="G13" s="25"/>
       <c r="H13" t="s">
         <v>69</v>
       </c>
@@ -3802,18 +3872,21 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B14" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="10" t="s">
         <v>122</v>
       </c>
+      <c r="G14" s="25"/>
       <c r="H14" t="s">
         <v>69</v>
       </c>
@@ -3828,18 +3901,21 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B15" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="10" t="s">
         <v>124</v>
       </c>
+      <c r="G15" s="25"/>
       <c r="H15" t="s">
         <v>69</v>
       </c>
@@ -3854,18 +3930,21 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="B16" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="10" t="s">
         <v>126</v>
       </c>
+      <c r="G16" s="25"/>
       <c r="H16" t="s">
         <v>69</v>
       </c>
@@ -3880,18 +3959,21 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B17" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="10" t="s">
         <v>128</v>
       </c>
+      <c r="G17" s="25"/>
       <c r="H17" t="s">
         <v>69</v>
       </c>
@@ -3906,63 +3988,128 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="B18" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="10" t="s">
         <v>131</v>
       </c>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="25" t="s">
         <v>584</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="B19" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25" t="s">
         <v>327</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="10" t="s">
         <v>585</v>
       </c>
+      <c r="G19" s="25"/>
       <c r="H19" t="s">
         <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="J19" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="K19" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>588</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="25" t="s">
+        <v>586</v>
+      </c>
+      <c r="B20" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E20" t="s">
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25" t="s">
         <v>328</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>589</v>
-      </c>
+      <c r="F20" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="G20" s="25"/>
       <c r="H20" t="s">
         <v>69</v>
       </c>
+      <c r="I20" t="s">
+        <v>596</v>
+      </c>
+      <c r="J20" t="s">
+        <v>597</v>
+      </c>
+      <c r="K20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>593</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>594</v>
+      </c>
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>590</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>587</v>
+      </c>
+      <c r="G22" s="25"/>
+      <c r="H22" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" t="s">
+        <v>591</v>
+      </c>
+      <c r="J22" t="s">
+        <v>592</v>
+      </c>
+      <c r="K22" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3977,2210 +4124,2210 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="14" width="15.0" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="14" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="14" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="14" width="10.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="14" width="73.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="14" width="9.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="14" width="11.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="14" width="19.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="14" width="13.140625" collapsed="true"/>
-    <col min="11" max="12" bestFit="true" customWidth="true" style="14" width="17.42578125" collapsed="true"/>
-    <col min="13" max="16384" style="14" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="13" width="15.0" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" style="13" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="10.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="13" width="73.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="13" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="13" width="11.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="13" width="19.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="13" width="13.140625" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" style="13" width="17.42578125" collapsed="true"/>
+    <col min="13" max="16384" style="13" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>377</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>378</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>427</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>429</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>430</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="13" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="B3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="14" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
+      <c r="B4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="14"/>
+      <c r="H4" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15" t="s">
+      <c r="B5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15" t="s">
+      <c r="B6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="14" t="s">
+      <c r="G6" s="14"/>
+      <c r="H6" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15" t="s">
+      <c r="B7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="14"/>
+      <c r="H7" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15" t="s">
+      <c r="B8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="14" t="s">
+      <c r="G8" s="14"/>
+      <c r="H8" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15" t="s">
+      <c r="B9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="14" t="s">
+      <c r="G9" s="14"/>
+      <c r="H9" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>375</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15" t="s">
+      <c r="B10" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="14" t="s">
+      <c r="G10" s="14"/>
+      <c r="H10" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15" t="s">
+      <c r="B11" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="14" t="s">
+      <c r="G11" s="14"/>
+      <c r="H11" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15" t="s">
+      <c r="B12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="14" t="s">
+      <c r="G12" s="14"/>
+      <c r="H12" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
+      <c r="B13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="14" t="s">
+      <c r="G13" s="14"/>
+      <c r="H13" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15" t="s">
+      <c r="B14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="14" t="s">
+      <c r="G14" s="14"/>
+      <c r="H14" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>358</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15" t="s">
+      <c r="B15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="14" t="s">
+      <c r="G15" s="14"/>
+      <c r="H15" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="K15" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15" t="s">
+      <c r="B16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="14" t="s">
+      <c r="G16" s="14"/>
+      <c r="H16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15" t="s">
+      <c r="B17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="14" t="s">
+      <c r="G17" s="14"/>
+      <c r="H17" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15" t="s">
+      <c r="B18" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="14" t="s">
+      <c r="G18" s="14"/>
+      <c r="H18" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="13" t="s">
         <v>365</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K18" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15" t="s">
+      <c r="B19" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="14" t="s">
+      <c r="G19" s="14"/>
+      <c r="H19" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="13" t="s">
         <v>379</v>
       </c>
-      <c r="K19" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="N19" s="14" t="s">
+      <c r="K19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N19" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15" t="s">
+      <c r="B20" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="14" t="s">
+      <c r="G20" s="14"/>
+      <c r="H20" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="13" t="s">
         <v>363</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15" t="s">
+      <c r="B21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="14" t="s">
+      <c r="G21" s="14"/>
+      <c r="H21" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15" t="s">
+      <c r="B22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="14" t="s">
+      <c r="G22" s="14"/>
+      <c r="H22" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15" t="s">
+      <c r="B23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="14" t="s">
+      <c r="G23" s="14"/>
+      <c r="H23" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="13" t="s">
         <v>434</v>
       </c>
-      <c r="K23" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L23" s="14" t="s">
+      <c r="K23" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="M23" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="N23" s="14" t="s">
+      <c r="N23" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="14" t="s">
+      <c r="O23" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15" t="s">
+      <c r="B24" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="14" t="s">
+      <c r="G24" s="14"/>
+      <c r="H24" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="13" t="s">
         <v>435</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="13" t="s">
         <v>436</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15" t="s">
+      <c r="B25" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="14">
         <v>4</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="I25" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="J25" s="13" t="s">
         <v>438</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="L25" s="14" t="s">
+      <c r="L25" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="M25" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="N25" s="14" t="s">
+      <c r="N25" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="O25" s="14" t="s">
+      <c r="O25" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B26" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15" t="s">
+      <c r="B26" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="14" t="s">
+      <c r="G26" s="14"/>
+      <c r="H26" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="J26" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="K26" s="14" t="s">
+      <c r="K26" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15" t="s">
+      <c r="B27" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="14">
         <v>4</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="13" t="s">
         <v>439</v>
       </c>
-      <c r="K27" s="14" t="s">
+      <c r="K27" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="L27" s="14" t="s">
+      <c r="L27" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="M27" s="14" t="s">
+      <c r="M27" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="N27" s="14" t="s">
+      <c r="N27" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="O27" s="14" t="s">
+      <c r="O27" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15" t="s">
+      <c r="B28" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="14" t="s">
+      <c r="G28" s="14"/>
+      <c r="H28" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="J28" s="14" t="s">
+      <c r="J28" s="13" t="s">
         <v>440</v>
       </c>
-      <c r="K28" s="14" t="s">
+      <c r="K28" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15" t="s">
+      <c r="B29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="14">
         <v>4</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="J29" s="14" t="s">
+      <c r="J29" s="13" t="s">
         <v>441</v>
       </c>
-      <c r="K29" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L29" s="14" t="s">
+      <c r="K29" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L29" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="M29" s="14" t="s">
+      <c r="M29" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="N29" s="14" t="s">
+      <c r="N29" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="O29" s="14" t="s">
+      <c r="O29" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B30" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15" t="s">
+      <c r="B30" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="16" t="s">
         <v>463</v>
       </c>
-      <c r="G30" s="15"/>
-      <c r="H30" s="14" t="s">
+      <c r="G30" s="14"/>
+      <c r="H30" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="J30" s="13" t="s">
         <v>334</v>
       </c>
-      <c r="K30" s="14" t="s">
+      <c r="K30" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15" t="s">
+      <c r="B31" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G31" s="14">
         <v>4</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="13" t="s">
         <v>442</v>
       </c>
-      <c r="K31" s="14" t="s">
+      <c r="K31" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="L31" s="14" t="s">
+      <c r="L31" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="M31" s="14" t="s">
+      <c r="M31" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="N31" s="14" t="s">
+      <c r="N31" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="O31" s="14" t="s">
+      <c r="O31" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15" t="s">
+      <c r="B32" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="G32" s="15"/>
-      <c r="H32" s="14" t="s">
+      <c r="G32" s="14"/>
+      <c r="H32" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="13" t="s">
         <v>443</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15" t="s">
+      <c r="B33" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="14">
         <v>4</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="13" t="s">
         <v>437</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="13" t="s">
         <v>444</v>
       </c>
-      <c r="K33" s="14" t="s">
+      <c r="K33" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="L33" s="14" t="s">
+      <c r="L33" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="M33" s="14" t="s">
+      <c r="M33" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="N33" s="14" t="s">
+      <c r="N33" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="O33" s="14" t="s">
+      <c r="O33" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15" t="s">
+      <c r="B34" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="16" t="s">
         <v>464</v>
       </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="14" t="s">
+      <c r="G34" s="14"/>
+      <c r="H34" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I34" s="14" t="s">
+      <c r="I34" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="K34" s="14" t="s">
+      <c r="K34" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15" t="s">
+      <c r="B35" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="16" t="s">
         <v>291</v>
       </c>
-      <c r="G35" s="15"/>
-      <c r="H35" s="14" t="s">
+      <c r="G35" s="14"/>
+      <c r="H35" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="13" t="s">
         <v>445</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="K35" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L35" s="14" t="s">
+      <c r="K35" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="M35" s="14" t="s">
+      <c r="M35" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="N35" s="14" t="s">
+      <c r="N35" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15" t="s">
+      <c r="B36" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="G36" s="15">
+      <c r="G36" s="14">
         <v>10</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="I36" s="13" t="s">
         <v>447</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="J36" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="K36" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="L36" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="M36" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="N36" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="O36" s="14" t="s">
+      <c r="K36" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M36" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N36" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="O36" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="P36" s="14" t="s">
+      <c r="P36" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="Q36" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="R36" s="14" t="s">
+      <c r="Q36" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="R36" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="S36" s="14" t="s">
+      <c r="S36" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="T36" s="14" t="s">
+      <c r="T36" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15" t="s">
+      <c r="B37" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="G37" s="15"/>
-      <c r="H37" s="14" t="s">
+      <c r="G37" s="14"/>
+      <c r="H37" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="J37" s="14" t="s">
+      <c r="J37" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="K37" s="14" t="s">
+      <c r="K37" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="B38" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15" t="s">
+      <c r="B38" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="F38" s="18" t="s">
+      <c r="F38" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="G38" s="15"/>
-      <c r="H38" s="14" t="s">
+      <c r="G38" s="14"/>
+      <c r="H38" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="K38" s="14" t="s">
+      <c r="K38" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15" t="s">
+      <c r="B39" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="F39" s="18" t="s">
+      <c r="F39" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="G39" s="15"/>
-      <c r="H39" s="14" t="s">
+      <c r="G39" s="14"/>
+      <c r="H39" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I39" s="14" t="s">
+      <c r="I39" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="J39" s="14" t="s">
+      <c r="J39" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="K39" s="14" t="s">
+      <c r="K39" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="B40" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15" t="s">
+      <c r="B40" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="G40" s="15"/>
-      <c r="H40" s="14" t="s">
+      <c r="G40" s="14"/>
+      <c r="H40" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="I40" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="J40" s="14" t="s">
+      <c r="J40" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="K40" s="14" t="s">
+      <c r="K40" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15" t="s">
+      <c r="B41" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F41" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="G41" s="15"/>
-      <c r="H41" s="14" t="s">
+      <c r="G41" s="14"/>
+      <c r="H41" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I41" s="14" t="s">
+      <c r="I41" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="J41" s="14" t="s">
+      <c r="J41" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="K41" s="14" t="s">
+      <c r="K41" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="B42" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15" t="s">
+      <c r="B42" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="G42" s="15"/>
-      <c r="H42" s="14" t="s">
+      <c r="G42" s="14"/>
+      <c r="H42" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I42" s="14" t="s">
+      <c r="I42" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="J42" s="14" t="s">
+      <c r="J42" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="K42" s="14" t="s">
+      <c r="K42" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15" t="s">
+      <c r="B43" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="G43" s="15"/>
-      <c r="H43" s="14" t="s">
+      <c r="G43" s="14"/>
+      <c r="H43" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I43" s="14" t="s">
+      <c r="I43" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="J43" s="14" t="s">
+      <c r="J43" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="K43" s="14" t="s">
+      <c r="K43" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15" t="s">
+      <c r="B44" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="F44" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="G44" s="15"/>
-      <c r="H44" s="14" t="s">
+      <c r="G44" s="14"/>
+      <c r="H44" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I44" s="14" t="s">
+      <c r="I44" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="J44" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="K44" s="14" t="s">
+      <c r="K44" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15" t="s">
+      <c r="B45" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="G45" s="15"/>
-      <c r="H45" s="14" t="s">
+      <c r="G45" s="14"/>
+      <c r="H45" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I45" s="14" t="s">
+      <c r="I45" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="J45" s="14" t="s">
+      <c r="J45" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="K45" s="14" t="s">
+      <c r="K45" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="B46" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15" t="s">
+      <c r="B46" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="G46" s="15"/>
-      <c r="H46" s="14" t="s">
+      <c r="G46" s="14"/>
+      <c r="H46" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I46" s="14" t="s">
+      <c r="I46" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="J46" s="14" t="s">
+      <c r="J46" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="K46" s="14" t="s">
+      <c r="K46" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15" t="s">
+      <c r="B47" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F47" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15" t="s">
+      <c r="B48" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F48" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="G48" s="15"/>
-      <c r="H48" s="14" t="s">
+      <c r="G48" s="14"/>
+      <c r="H48" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I48" s="14" t="s">
+      <c r="I48" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="J48" s="14" t="s">
+      <c r="J48" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="K48" s="14" t="s">
+      <c r="K48" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="B49" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15" t="s">
+      <c r="B49" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F49" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15" t="s">
+      <c r="B50" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F50" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
-      <c r="K50" s="15"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="B51" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15" t="s">
+      <c r="B51" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B52" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15" t="s">
+      <c r="B52" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F52" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="B53" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15" t="s">
+      <c r="B53" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F53" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="B54" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15" t="s">
+      <c r="B54" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F54" s="16" t="s">
         <v>263</v>
       </c>
-      <c r="G54" s="15"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B55" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15" t="s">
+      <c r="B55" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="F55" s="17" t="s">
+      <c r="F55" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15" t="s">
+      <c r="G55" s="14"/>
+      <c r="H55" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I55" s="15" t="s">
+      <c r="I55" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="J55" s="15" t="s">
+      <c r="J55" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="K55" s="15" t="s">
+      <c r="K55" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="B56" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15" t="s">
+      <c r="B56" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="F56" s="17" t="s">
+      <c r="F56" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="G56" s="15"/>
-      <c r="H56" s="15" t="s">
+      <c r="G56" s="14"/>
+      <c r="H56" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I56" s="15" t="s">
+      <c r="I56" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="J56" s="15" t="s">
+      <c r="J56" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="K56" s="15" t="s">
+      <c r="K56" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="B57" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15" t="s">
+      <c r="B57" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="F57" s="17" t="s">
+      <c r="F57" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15" t="s">
+      <c r="G57" s="14"/>
+      <c r="H57" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I57" s="15" t="s">
+      <c r="I57" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="J57" s="15" t="s">
+      <c r="J57" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="K57" s="15" t="s">
+      <c r="K57" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="B58" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15" t="s">
+      <c r="B58" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="F58" s="17" t="s">
+      <c r="F58" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="B59" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19" t="s">
+      <c r="B59" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="F59" s="20" t="s">
+      <c r="F59" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15" t="s">
+      <c r="B60" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="F60" s="17" t="s">
+      <c r="F60" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B61" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15" t="s">
+      <c r="B61" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="F61" s="18" t="s">
+      <c r="F61" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="G61" s="15"/>
-      <c r="H61" s="15" t="s">
+      <c r="G61" s="14"/>
+      <c r="H61" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I61" s="15" t="s">
+      <c r="I61" s="14" t="s">
         <v>453</v>
       </c>
-      <c r="J61" s="15" t="s">
+      <c r="J61" s="14" t="s">
         <v>454</v>
       </c>
-      <c r="K61" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L61" s="15"/>
+      <c r="K61" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L61" s="14"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="B62" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15" t="s">
+      <c r="B62" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F62" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15" t="s">
+      <c r="G62" s="14"/>
+      <c r="H62" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I62" s="15" t="s">
+      <c r="I62" s="14" t="s">
         <v>453</v>
       </c>
-      <c r="J62" s="15" t="s">
+      <c r="J62" s="14" t="s">
         <v>455</v>
       </c>
-      <c r="K62" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L62" s="15"/>
+      <c r="K62" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L62" s="14"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="B63" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15" t="s">
+      <c r="B63" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="F63" s="18" t="s">
+      <c r="F63" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="G63" s="15"/>
-      <c r="H63" s="15" t="s">
+      <c r="G63" s="14"/>
+      <c r="H63" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I63" s="15" t="s">
+      <c r="I63" s="14" t="s">
         <v>456</v>
       </c>
-      <c r="J63" s="15" t="s">
+      <c r="J63" s="14" t="s">
         <v>457</v>
       </c>
-      <c r="K63" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L63" s="15"/>
+      <c r="K63" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L63" s="14"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="B64" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15" t="s">
+      <c r="B64" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="F64" s="18" t="s">
+      <c r="F64" s="17" t="s">
         <v>452</v>
       </c>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15" t="s">
+      <c r="G64" s="14"/>
+      <c r="H64" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I64" s="15" t="s">
+      <c r="I64" s="14" t="s">
         <v>460</v>
       </c>
-      <c r="J64" s="15" t="s">
+      <c r="J64" s="14" t="s">
         <v>461</v>
       </c>
-      <c r="K64" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L64" s="15"/>
+      <c r="K64" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L64" s="14"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="B65" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="15" t="s">
+      <c r="B65" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="F65" s="18" t="s">
+      <c r="F65" s="17" t="s">
         <v>451</v>
       </c>
-      <c r="G65" s="15"/>
-      <c r="H65" s="15" t="s">
+      <c r="G65" s="14"/>
+      <c r="H65" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I65" s="15" t="s">
+      <c r="I65" s="14" t="s">
         <v>458</v>
       </c>
-      <c r="J65" s="15" t="s">
+      <c r="J65" s="14" t="s">
         <v>459</v>
       </c>
-      <c r="K65" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L65" s="15"/>
+      <c r="K65" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L65" s="14"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="B66" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15" t="s">
+      <c r="B66" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="F66" s="18" t="s">
+      <c r="F66" s="17" t="s">
         <v>317</v>
       </c>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" s="15" t="s">
+      <c r="A67" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="B67" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15" t="s">
+      <c r="B67" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="F67" s="18" t="s">
+      <c r="F67" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="G67" s="15"/>
-      <c r="H67" s="15" t="s">
+      <c r="G67" s="14"/>
+      <c r="H67" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I67" s="15" t="s">
+      <c r="I67" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="J67" s="15" t="s">
+      <c r="J67" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="K67" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L67" s="15"/>
+      <c r="K67" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L67" s="14"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A68" s="15" t="s">
+      <c r="A68" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B68" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="21" t="s">
+      <c r="B68" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="F68" s="18" t="s">
+      <c r="F68" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="G68" s="15"/>
-      <c r="H68" s="15" t="s">
+      <c r="G68" s="14"/>
+      <c r="H68" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I68" s="15" t="s">
+      <c r="I68" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="J68" s="15" t="s">
+      <c r="J68" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="K68" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L68" s="15"/>
+      <c r="K68" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L68" s="14"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="B69" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="21" t="s">
+      <c r="B69" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="F69" s="18" t="s">
+      <c r="F69" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="G69" s="15"/>
-      <c r="H69" s="15" t="s">
+      <c r="G69" s="14"/>
+      <c r="H69" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I69" s="15" t="s">
+      <c r="I69" s="14" t="s">
         <v>533</v>
       </c>
-      <c r="J69" s="15" t="s">
+      <c r="J69" s="14" t="s">
         <v>534</v>
       </c>
-      <c r="K69" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L69" s="15"/>
+      <c r="K69" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L69" s="14"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A70" s="15" t="s">
+      <c r="A70" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="B70" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="21" t="s">
+      <c r="B70" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="F70" s="18" t="s">
+      <c r="F70" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="G70" s="15"/>
-      <c r="H70" s="15" t="s">
+      <c r="G70" s="14"/>
+      <c r="H70" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I70" s="15" t="s">
+      <c r="I70" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="J70" s="15" t="s">
+      <c r="J70" s="14" t="s">
         <v>466</v>
       </c>
-      <c r="K70" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L70" s="15"/>
+      <c r="K70" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L70" s="14"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="B71" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="15"/>
-      <c r="E71" s="21" t="s">
+      <c r="B71" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="F71" s="18" t="s">
+      <c r="F71" s="17" t="s">
         <v>462</v>
       </c>
-      <c r="G71" s="15"/>
-      <c r="H71" s="15" t="s">
+      <c r="G71" s="14"/>
+      <c r="H71" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I71" s="15" t="s">
+      <c r="I71" s="14" t="s">
         <v>533</v>
       </c>
-      <c r="J71" s="15" t="s">
+      <c r="J71" s="14" t="s">
         <v>535</v>
       </c>
-      <c r="K71" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L71" s="15"/>
+      <c r="K71" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L71" s="14"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" s="15" t="s">
+      <c r="A72" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="B72" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
-      <c r="E72" s="21" t="s">
+      <c r="B72" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="F72" s="18" t="s">
+      <c r="F72" s="17" t="s">
         <v>322</v>
       </c>
-      <c r="G72" s="15"/>
-      <c r="H72" s="15" t="s">
+      <c r="G72" s="14"/>
+      <c r="H72" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I72" s="15" t="s">
+      <c r="I72" s="14" t="s">
         <v>465</v>
       </c>
-      <c r="J72" s="15" t="s">
+      <c r="J72" s="14" t="s">
         <v>467</v>
       </c>
-      <c r="K72" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L72" s="15"/>
+      <c r="K72" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L72" s="14"/>
     </row>
     <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+      <c r="A73" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="B73" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="22" t="s">
+      <c r="B73" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="F73" s="18" t="s">
+      <c r="F73" s="17" t="s">
         <v>323</v>
       </c>
-      <c r="G73" s="15"/>
+      <c r="G73" s="14"/>
       <c r="H73" t="s">
         <v>69</v>
       </c>
@@ -6193,54 +6340,54 @@
       <c r="K73" t="s">
         <v>70</v>
       </c>
-      <c r="L73" s="15"/>
+      <c r="L73" s="14"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A74" s="15" t="s">
+      <c r="A74" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="B74" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="21" t="s">
+      <c r="B74" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="F74" s="18" t="s">
+      <c r="F74" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="G74" s="15"/>
-      <c r="H74" s="15" t="s">
+      <c r="G74" s="14"/>
+      <c r="H74" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I74" s="15" t="s">
+      <c r="I74" s="14" t="s">
         <v>503</v>
       </c>
-      <c r="J74" s="15" t="s">
+      <c r="J74" s="14" t="s">
         <v>504</v>
       </c>
-      <c r="K74" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="L74" s="15"/>
+      <c r="K74" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L74" s="14"/>
     </row>
     <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
+      <c r="A75" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="B75" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="21" t="s">
+      <c r="B75" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="F75" s="18" t="s">
+      <c r="F75" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="G75" s="15"/>
+      <c r="G75" s="14"/>
       <c r="H75" t="s">
         <v>69</v>
       </c>
@@ -6253,24 +6400,24 @@
       <c r="K75" t="s">
         <v>70</v>
       </c>
-      <c r="L75" s="15"/>
+      <c r="L75" s="14"/>
     </row>
     <row r="76" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
+      <c r="A76" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="15" t="s">
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="F76" s="18" t="s">
+      <c r="F76" s="17" t="s">
         <v>532</v>
       </c>
-      <c r="G76" s="15"/>
+      <c r="G76" s="14"/>
       <c r="H76" t="s">
         <v>69</v>
       </c>
@@ -6283,24 +6430,24 @@
       <c r="K76" t="s">
         <v>70</v>
       </c>
-      <c r="L76" s="15"/>
+      <c r="L76" s="14"/>
     </row>
     <row r="77" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+      <c r="A77" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B77" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="15" t="s">
+      <c r="B77" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="F77" s="18" t="s">
+      <c r="F77" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="G77" s="15"/>
+      <c r="G77" s="14"/>
       <c r="H77" t="s">
         <v>69</v>
       </c>
@@ -6313,293 +6460,293 @@
       <c r="K77" t="s">
         <v>70</v>
       </c>
-      <c r="L77" s="15"/>
+      <c r="L77" s="14"/>
     </row>
     <row r="78" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A78" s="15" t="s">
+      <c r="A78" s="14" t="s">
         <v>536</v>
       </c>
-      <c r="B78" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="15" t="s">
+      <c r="B78" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14" t="s">
         <v>537</v>
       </c>
-      <c r="F78" s="18" t="s">
+      <c r="F78" s="17" t="s">
         <v>554</v>
       </c>
-      <c r="G78" s="15"/>
-      <c r="H78" s="15"/>
-      <c r="I78" s="15"/>
-      <c r="J78" s="15"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="15"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
     </row>
     <row r="79" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="14" t="s">
         <v>538</v>
       </c>
-      <c r="B79" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="15" t="s">
+      <c r="B79" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14" t="s">
         <v>539</v>
       </c>
-      <c r="F79" s="18" t="s">
+      <c r="F79" s="17" t="s">
         <v>555</v>
       </c>
-      <c r="G79" s="15"/>
-      <c r="H79" s="15"/>
-      <c r="I79" s="15"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="15"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
     </row>
     <row r="80" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A80" s="15" t="s">
+      <c r="A80" s="14" t="s">
         <v>540</v>
       </c>
-      <c r="B80" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15"/>
-      <c r="E80" s="15" t="s">
+      <c r="B80" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="F80" s="18" t="s">
+      <c r="F80" s="17" t="s">
         <v>556</v>
       </c>
-      <c r="G80" s="15"/>
-      <c r="H80" s="15"/>
-      <c r="I80" s="15"/>
-      <c r="J80" s="15"/>
-      <c r="K80" s="15"/>
-      <c r="L80" s="15"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A81" s="15" t="s">
+      <c r="A81" s="14" t="s">
         <v>542</v>
       </c>
-      <c r="B81" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15" t="s">
+      <c r="B81" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14" t="s">
         <v>543</v>
       </c>
-      <c r="F81" s="18" t="s">
+      <c r="F81" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="G81" s="15"/>
-      <c r="H81" s="15"/>
-      <c r="I81" s="15"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="15"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A82" s="15" t="s">
+      <c r="A82" s="14" t="s">
         <v>544</v>
       </c>
-      <c r="B82" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="15" t="s">
+      <c r="B82" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14" t="s">
         <v>545</v>
       </c>
-      <c r="F82" s="18" t="s">
+      <c r="F82" s="17" t="s">
         <v>558</v>
       </c>
-      <c r="G82" s="15"/>
-      <c r="H82" s="15"/>
-      <c r="I82" s="15"/>
-      <c r="J82" s="15"/>
-      <c r="K82" s="15"/>
-      <c r="L82" s="15"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A83" s="15" t="s">
+      <c r="A83" s="14" t="s">
         <v>546</v>
       </c>
-      <c r="B83" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="15" t="s">
+      <c r="B83" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14" t="s">
         <v>547</v>
       </c>
-      <c r="F83" s="18" t="s">
+      <c r="F83" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="15"/>
-      <c r="J83" s="15"/>
-      <c r="K83" s="15"/>
-      <c r="L83" s="15"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A84" s="15" t="s">
+      <c r="A84" s="14" t="s">
         <v>548</v>
       </c>
-      <c r="B84" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="15"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="15" t="s">
+      <c r="B84" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14" t="s">
         <v>549</v>
       </c>
-      <c r="F84" s="18" t="s">
+      <c r="F84" s="17" t="s">
         <v>560</v>
       </c>
-      <c r="G84" s="15"/>
-      <c r="H84" s="15"/>
-      <c r="I84" s="15"/>
-      <c r="J84" s="15"/>
-      <c r="K84" s="15"/>
-      <c r="L84" s="15"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A85" s="15" t="s">
+      <c r="A85" s="14" t="s">
         <v>550</v>
       </c>
-      <c r="B85" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="15" t="s">
+      <c r="B85" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14" t="s">
         <v>551</v>
       </c>
-      <c r="F85" s="18" t="s">
+      <c r="F85" s="17" t="s">
         <v>561</v>
       </c>
-      <c r="G85" s="15"/>
-      <c r="H85" s="15"/>
-      <c r="I85" s="15"/>
-      <c r="J85" s="15"/>
-      <c r="K85" s="15"/>
-      <c r="L85" s="15"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A86" s="15" t="s">
+      <c r="A86" s="14" t="s">
         <v>552</v>
       </c>
-      <c r="B86" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" s="15"/>
-      <c r="D86" s="15"/>
-      <c r="E86" s="15" t="s">
+      <c r="B86" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14" t="s">
         <v>553</v>
       </c>
-      <c r="F86" s="18" t="s">
+      <c r="F86" s="17" t="s">
         <v>562</v>
       </c>
-      <c r="G86" s="15"/>
-      <c r="H86" s="15"/>
-      <c r="I86" s="15"/>
-      <c r="J86" s="15"/>
-      <c r="K86" s="15"/>
-      <c r="L86" s="15"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A87" s="15" t="s">
+      <c r="A87" s="14" t="s">
         <v>572</v>
       </c>
-      <c r="B87" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C87" s="15"/>
-      <c r="D87" s="15"/>
-      <c r="E87" s="15" t="s">
+      <c r="B87" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14" t="s">
         <v>573</v>
       </c>
-      <c r="F87" s="18" t="s">
+      <c r="F87" s="17" t="s">
         <v>574</v>
       </c>
-      <c r="G87" s="15"/>
-      <c r="H87" s="15"/>
-      <c r="I87" s="15"/>
-      <c r="J87" s="15"/>
-      <c r="K87" s="15"/>
-      <c r="L87" s="15"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A88" s="15" t="s">
+      <c r="A88" s="14" t="s">
         <v>575</v>
       </c>
-      <c r="B88" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C88" s="15"/>
-      <c r="D88" s="15"/>
-      <c r="E88" s="15" t="s">
+      <c r="B88" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14" t="s">
         <v>576</v>
       </c>
-      <c r="F88" s="18" t="s">
+      <c r="F88" s="17" t="s">
         <v>577</v>
       </c>
-      <c r="G88" s="15"/>
-      <c r="H88" s="15"/>
-      <c r="I88" s="15"/>
-      <c r="J88" s="15"/>
-      <c r="K88" s="15"/>
-      <c r="L88" s="15"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A89" s="15" t="s">
+      <c r="A89" s="14" t="s">
         <v>578</v>
       </c>
-      <c r="B89" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15" t="s">
+      <c r="B89" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14" t="s">
         <v>579</v>
       </c>
-      <c r="F89" s="18" t="s">
+      <c r="F89" s="17" t="s">
         <v>580</v>
       </c>
-      <c r="G89" s="15"/>
-      <c r="H89" s="15"/>
-      <c r="I89" s="15"/>
-      <c r="J89" s="15"/>
-      <c r="K89" s="15"/>
-      <c r="L89" s="15"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A90" s="15" t="s">
+      <c r="A90" s="14" t="s">
         <v>581</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B90" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15" t="s">
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14" t="s">
         <v>582</v>
       </c>
-      <c r="F90" s="18" t="s">
+      <c r="F90" s="17" t="s">
         <v>583</v>
       </c>
-      <c r="G90" s="15"/>
-      <c r="H90" s="15"/>
-      <c r="I90" s="15"/>
-      <c r="J90" s="15"/>
-      <c r="K90" s="15"/>
-      <c r="L90" s="15"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>